<commit_message>
adding anonymized team code
</commit_message>
<xml_diff>
--- a/results/dataout_print.xlsx
+++ b/results/dataout_print.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6885" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6890" windowHeight="6120"/>
   </bookViews>
   <sheets>
     <sheet name="dataout" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="129">
   <si>
     <t>Sources of Variability</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Recoded missing on income to zero, elected not to counterfactual as this is a plausible (although highly controversial) procedural step</t>
-  </si>
-  <si>
-    <t>Some cases dropped due to matching the (unrelated) ID variable between waves</t>
   </si>
   <si>
     <t>A</t>
@@ -415,6 +412,12 @@
       </rPr>
       <t>deal example of the PIs being unable to find the exact mismatch within three hours of work).</t>
     </r>
+  </si>
+  <si>
+    <t>Used a different 13 country-sample based on data availability at the country-level and highest 13 scores on the social spending indicator, rather than select based on the individual-level data. Instructions were not perfectly clear, but this led to an unbalanced time-series with some of the 13 countries having only one wave in either 1996 or 2006.</t>
+  </si>
+  <si>
+    <t>Interpretational</t>
   </si>
 </sst>
 </file>
@@ -1141,13 +1144,13 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1473,91 +1476,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R175"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A115" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A82" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="38" customWidth="1"/>
-    <col min="5" max="6" width="7.5703125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="38" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="30" customWidth="1"/>
-    <col min="9" max="9" width="46.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" style="37" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" style="38" customWidth="1"/>
+    <col min="5" max="6" width="7.54296875" style="37" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" style="38" customWidth="1"/>
+    <col min="8" max="8" width="2.26953125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="46.81640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.1796875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C2" s="62" t="s">
+    <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C2" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="63"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="62"/>
-    </row>
-    <row r="3" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G2" s="63"/>
+    </row>
+    <row r="3" spans="1:18" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="D3" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="G3" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q3" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R3" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="23">
         <v>3</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>9</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="46.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23">
         <v>10</v>
       </c>
@@ -1679,13 +1682,13 @@
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="Q7" s="2">
         <v>12</v>
@@ -1694,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="97.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="97.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23"/>
       <c r="B8" s="24"/>
       <c r="C8" s="25"/>
@@ -1704,16 +1707,16 @@
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
       <c r="I8" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>15</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="23">
         <v>16</v>
       </c>
@@ -1778,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="34.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>17</v>
       </c>
@@ -1801,13 +1804,13 @@
         <v>3.2916666666666498E-3</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q11" s="2">
         <v>21</v>
@@ -1816,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="23">
         <v>19</v>
       </c>
@@ -1849,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>21</v>
       </c>
@@ -1881,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="23">
         <v>25</v>
       </c>
@@ -1905,13 +1908,13 @@
       </c>
       <c r="H14" s="27"/>
       <c r="I14" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q14" s="2">
         <v>31</v>
@@ -1920,7 +1923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="23"/>
       <c r="B15" s="24"/>
       <c r="C15" s="25"/>
@@ -1930,13 +1933,13 @@
       <c r="G15" s="26"/>
       <c r="H15" s="27"/>
       <c r="I15" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q15" s="2">
         <v>31</v>
@@ -1945,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
@@ -1955,13 +1958,13 @@
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
       <c r="I16" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q16" s="2">
         <v>31</v>
@@ -1970,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>29</v>
       </c>
@@ -2002,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A18" s="23">
         <v>31</v>
       </c>
@@ -2026,13 +2029,13 @@
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J18" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="Q18" s="2">
         <v>37</v>
@@ -2041,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A19" s="23"/>
       <c r="B19" s="24"/>
       <c r="C19" s="25"/>
@@ -2051,13 +2054,13 @@
       <c r="G19" s="26"/>
       <c r="H19" s="27"/>
       <c r="I19" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q19" s="2">
         <v>37</v>
@@ -2066,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>34</v>
       </c>
@@ -2093,10 +2096,10 @@
         <v>2</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q20" s="2">
         <v>40</v>
@@ -2105,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="23">
         <v>36</v>
       </c>
@@ -2138,68 +2141,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="63" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="63"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C23" s="62" t="s">
+    <row r="22" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C23" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="63"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="62"/>
-    </row>
-    <row r="24" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G23" s="63"/>
+    </row>
+    <row r="24" spans="1:18" ht="26" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H24" s="31"/>
       <c r="I24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q24" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R24" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>37</v>
       </c>
@@ -2225,10 +2228,10 @@
         <v>3</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q25" s="2">
         <v>43</v>
@@ -2237,15 +2240,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I26" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q26" s="2">
         <v>43</v>
@@ -2254,15 +2257,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I27" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q27" s="2">
         <v>43</v>
@@ -2271,15 +2274,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I28" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q28" s="2">
         <v>43</v>
@@ -2288,13 +2291,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I29" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q29" s="2">
         <v>43</v>
@@ -2303,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" s="23">
         <v>38</v>
       </c>
@@ -2336,7 +2339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>39</v>
       </c>
@@ -2359,13 +2362,13 @@
         <v>7.1666666666666502E-3</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q31" s="2">
         <v>46</v>
@@ -2374,15 +2377,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I32" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q32" s="2">
         <v>46</v>
@@ -2391,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="23">
         <v>40</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>41</v>
       </c>
@@ -2447,13 +2450,13 @@
         <v>7.6458333333333295E-2</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q34" s="2">
         <v>48</v>
@@ -2462,15 +2465,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I35" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q35" s="2">
         <v>48</v>
@@ -2479,15 +2482,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I36" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q36" s="2">
         <v>48</v>
@@ -2496,15 +2499,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I37" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q37" s="2">
         <v>48</v>
@@ -2513,7 +2516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" s="23">
         <v>42</v>
       </c>
@@ -2546,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>44</v>
       </c>
@@ -2579,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A40" s="23">
         <v>45</v>
       </c>
@@ -2603,13 +2606,13 @@
       </c>
       <c r="H40" s="27"/>
       <c r="I40" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J40" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J40" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="K40" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q40" s="2">
         <v>53</v>
@@ -2618,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:18" s="58" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="58">
         <v>47</v>
       </c>
@@ -2651,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>48</v>
       </c>
@@ -2675,13 +2678,13 @@
       </c>
       <c r="H42" s="36"/>
       <c r="I42" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J42" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K42" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="K42" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="Q42" s="2">
         <v>57</v>
@@ -2690,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="33"/>
       <c r="C43" s="34"/>
@@ -2700,13 +2703,13 @@
       <c r="G43" s="35"/>
       <c r="H43" s="36"/>
       <c r="I43" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q43" s="2">
         <v>57</v>
@@ -2715,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A44" s="23">
         <v>53</v>
       </c>
@@ -2739,13 +2742,13 @@
       </c>
       <c r="H44" s="27"/>
       <c r="I44" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q44" s="2">
         <v>62</v>
@@ -2754,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" s="23"/>
       <c r="B45" s="24"/>
       <c r="C45" s="25"/>
@@ -2767,68 +2770,68 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="63" t="s">
-        <v>114</v>
-      </c>
-      <c r="B46" s="63"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="63"/>
-      <c r="K46" s="63"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C47" s="62" t="s">
+    <row r="46" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C47" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="63"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="62"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G47" s="62"/>
-    </row>
-    <row r="48" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G47" s="63"/>
+    </row>
+    <row r="48" spans="1:18" ht="26" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G48" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H48" s="31"/>
       <c r="I48" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q48" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R48" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" ht="67.5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="46" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>56</v>
       </c>
@@ -2852,13 +2855,13 @@
       </c>
       <c r="H49" s="36"/>
       <c r="I49" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q49" s="2">
         <v>67</v>
@@ -2867,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A50" s="23">
         <v>60</v>
       </c>
@@ -2891,13 +2894,13 @@
       </c>
       <c r="H50" s="27"/>
       <c r="I50" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q50" s="2">
         <v>72</v>
@@ -2906,7 +2909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A51" s="40">
         <v>61</v>
       </c>
@@ -2939,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A52" s="23">
         <v>63</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>64</v>
       </c>
@@ -3005,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="23">
         <v>65</v>
       </c>
@@ -3029,13 +3032,13 @@
       </c>
       <c r="H54" s="27"/>
       <c r="I54" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K54" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q54" s="2">
         <v>77</v>
@@ -3044,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>66</v>
       </c>
@@ -3071,10 +3074,10 @@
         <v>1</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q55" s="2">
         <v>79</v>
@@ -3083,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="33"/>
       <c r="C56" s="34"/>
@@ -3096,10 +3099,10 @@
         <v>2</v>
       </c>
       <c r="J56" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q56" s="2">
         <v>79</v>
@@ -3108,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="33"/>
       <c r="C57" s="34"/>
@@ -3118,13 +3121,13 @@
       <c r="G57" s="35"/>
       <c r="H57" s="36"/>
       <c r="I57" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q57" s="2">
         <v>79</v>
@@ -3133,7 +3136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="33"/>
       <c r="C58" s="34"/>
@@ -3143,13 +3146,13 @@
       <c r="G58" s="35"/>
       <c r="H58" s="36"/>
       <c r="I58" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q58" s="2">
         <v>79</v>
@@ -3158,7 +3161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A59" s="23">
         <v>70</v>
       </c>
@@ -3182,13 +3185,13 @@
       </c>
       <c r="H59" s="27"/>
       <c r="I59" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K59" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q59" s="2">
         <v>84</v>
@@ -3197,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>71</v>
       </c>
@@ -3229,7 +3232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A61" s="23">
         <v>72</v>
       </c>
@@ -3253,13 +3256,13 @@
       </c>
       <c r="H61" s="27"/>
       <c r="I61" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K61" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q61" s="2">
         <v>87</v>
@@ -3268,7 +3271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="23"/>
       <c r="B62" s="24"/>
       <c r="C62" s="25"/>
@@ -3278,13 +3281,13 @@
       <c r="G62" s="26"/>
       <c r="H62" s="27"/>
       <c r="I62" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K62" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q62" s="2">
         <v>87</v>
@@ -3293,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>73</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:18" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="23">
         <v>76</v>
       </c>
@@ -3350,7 +3353,7 @@
       </c>
       <c r="H64" s="27"/>
       <c r="I64" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
@@ -3361,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>78</v>
       </c>
@@ -3394,7 +3397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="45">
         <v>82</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
       <c r="B67" s="33"/>
       <c r="C67" s="34"/>
@@ -3440,7 +3443,7 @@
       <c r="J67" s="8"/>
       <c r="K67" s="3"/>
     </row>
-    <row r="68" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="33"/>
       <c r="C68" s="34"/>
@@ -3453,7 +3456,7 @@
       <c r="J68" s="8"/>
       <c r="K68" s="3"/>
     </row>
-    <row r="69" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
       <c r="B69" s="33"/>
       <c r="C69" s="34"/>
@@ -3466,7 +3469,7 @@
       <c r="J69" s="8"/>
       <c r="K69" s="3"/>
     </row>
-    <row r="70" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="33"/>
       <c r="C70" s="34"/>
@@ -3479,7 +3482,7 @@
       <c r="J70" s="8"/>
       <c r="K70" s="3"/>
     </row>
-    <row r="71" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="33"/>
       <c r="C71" s="34"/>
@@ -3492,7 +3495,7 @@
       <c r="J71" s="8"/>
       <c r="K71" s="3"/>
     </row>
-    <row r="72" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="3"/>
       <c r="B72" s="33"/>
       <c r="C72" s="34"/>
@@ -3505,68 +3508,68 @@
       <c r="J72" s="8"/>
       <c r="K72" s="3"/>
     </row>
-    <row r="73" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="B73" s="61"/>
-      <c r="C73" s="61"/>
-      <c r="D73" s="61"/>
-      <c r="E73" s="61"/>
-      <c r="F73" s="61"/>
-      <c r="G73" s="61"/>
-      <c r="H73" s="61"/>
-      <c r="I73" s="61"/>
-      <c r="J73" s="61"/>
-      <c r="K73" s="61"/>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C74" s="62" t="s">
+    <row r="73" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73" s="62"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
+      <c r="H73" s="62"/>
+      <c r="I73" s="62"/>
+      <c r="J73" s="62"/>
+      <c r="K73" s="62"/>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C74" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D74" s="63"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D74" s="62"/>
-      <c r="E74" s="29"/>
-      <c r="F74" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G74" s="62"/>
-    </row>
-    <row r="75" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G74" s="63"/>
+    </row>
+    <row r="75" spans="1:18" ht="26" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D75" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G75" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H75" s="31"/>
       <c r="I75" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q75" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R75" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>1</v>
       </c>
@@ -3589,19 +3592,19 @@
         <v>2.37499999999999E-3</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q76" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="23">
         <v>4</v>
       </c>
@@ -3628,16 +3631,16 @@
         <v>1</v>
       </c>
       <c r="J77" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K77" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q77" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A78" s="23"/>
       <c r="B78" s="24"/>
       <c r="C78" s="25"/>
@@ -3647,19 +3650,19 @@
       <c r="G78" s="26"/>
       <c r="H78" s="27"/>
       <c r="I78" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J78" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K78" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q78" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>5</v>
       </c>
@@ -3682,47 +3685,47 @@
         <v>6.2999999999999801E-3</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q79" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I80" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q80" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I81" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q81" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A82" s="23">
         <v>6</v>
       </c>
@@ -3746,19 +3749,19 @@
       </c>
       <c r="H82" s="27"/>
       <c r="I82" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J82" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K82" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q82" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A83" s="23"/>
       <c r="B83" s="24"/>
       <c r="C83" s="25"/>
@@ -3768,19 +3771,19 @@
       <c r="G83" s="26"/>
       <c r="H83" s="27"/>
       <c r="I83" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J83" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K83" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q83" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>7</v>
       </c>
@@ -3803,33 +3806,33 @@
         <v>3.5297297297297199E-2</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J84" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q84" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I85" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q85" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A86" s="23">
         <v>8</v>
       </c>
@@ -3853,19 +3856,19 @@
       </c>
       <c r="H86" s="27"/>
       <c r="I86" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J86" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K86" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q86" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A87" s="23"/>
       <c r="B87" s="24"/>
       <c r="C87" s="25"/>
@@ -3875,19 +3878,19 @@
       <c r="G87" s="26"/>
       <c r="H87" s="27"/>
       <c r="I87" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K87" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q87" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>11</v>
       </c>
@@ -3910,69 +3913,74 @@
         <v>1.9E-2</v>
       </c>
       <c r="I88" s="6" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="J88" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q88" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="I89" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J89" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K89" s="6" t="s">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A89" s="23">
+        <v>12</v>
+      </c>
+      <c r="B89" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="C89" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="D89" s="26">
+        <v>6.4399999999999999E-2</v>
+      </c>
+      <c r="E89" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="F89" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="G89" s="26">
+        <v>6.4399999999999999E-2</v>
+      </c>
+      <c r="H89" s="27"/>
+      <c r="I89" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J89" s="7" t="s">
         <v>102</v>
       </c>
+      <c r="K89" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="Q89" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="23">
-        <v>12</v>
-      </c>
-      <c r="B90" s="24">
-        <v>0.8</v>
-      </c>
-      <c r="C90" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="D90" s="26">
-        <v>6.4399999999999999E-2</v>
-      </c>
-      <c r="E90" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="F90" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="G90" s="26">
-        <v>6.4399999999999999E-2</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="23"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="26"/>
       <c r="H90" s="27"/>
       <c r="I90" s="7" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="K90" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q90" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A91" s="23"/>
       <c r="B91" s="24"/>
       <c r="C91" s="25"/>
@@ -3982,19 +3990,19 @@
       <c r="G91" s="26"/>
       <c r="H91" s="27"/>
       <c r="I91" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J91" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K91" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q91" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>13</v>
       </c>
@@ -4017,85 +4025,85 @@
         <v>6.4749999999999903E-3</v>
       </c>
       <c r="I92" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J92" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K92" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q92" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I93" s="6"/>
       <c r="J93" s="8"/>
       <c r="K93" s="6"/>
     </row>
-    <row r="94" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="B94" s="61"/>
-      <c r="C94" s="61"/>
-      <c r="D94" s="61"/>
-      <c r="E94" s="61"/>
-      <c r="F94" s="61"/>
-      <c r="G94" s="61"/>
-      <c r="H94" s="61"/>
-      <c r="I94" s="61"/>
-      <c r="J94" s="61"/>
-      <c r="K94" s="61"/>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C95" s="62" t="s">
+    <row r="94" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A94" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B94" s="62"/>
+      <c r="C94" s="62"/>
+      <c r="D94" s="62"/>
+      <c r="E94" s="62"/>
+      <c r="F94" s="62"/>
+      <c r="G94" s="62"/>
+      <c r="H94" s="62"/>
+      <c r="I94" s="62"/>
+      <c r="J94" s="62"/>
+      <c r="K94" s="62"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C95" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D95" s="63"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D95" s="62"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G95" s="62"/>
-    </row>
-    <row r="96" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G95" s="63"/>
+    </row>
+    <row r="96" spans="1:18" ht="26" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D96" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G96" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H96" s="31"/>
       <c r="I96" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q96" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R96" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="23">
         <v>14</v>
       </c>
@@ -4119,19 +4127,19 @@
       </c>
       <c r="H97" s="27"/>
       <c r="I97" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J97" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K97" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q97" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>18</v>
       </c>
@@ -4155,19 +4163,19 @@
       </c>
       <c r="H98" s="36"/>
       <c r="I98" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J98" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K98" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q98" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A99" s="3"/>
       <c r="B99" s="33"/>
       <c r="C99" s="34"/>
@@ -4177,19 +4185,19 @@
       <c r="G99" s="35"/>
       <c r="H99" s="36"/>
       <c r="I99" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J99" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K99" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q99" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A100" s="23">
         <v>20</v>
       </c>
@@ -4216,16 +4224,16 @@
         <v>1</v>
       </c>
       <c r="J100" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K100" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q100" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A101" s="50"/>
       <c r="B101" s="51"/>
       <c r="C101" s="52"/>
@@ -4235,19 +4243,19 @@
       <c r="G101" s="53"/>
       <c r="H101" s="54"/>
       <c r="I101" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K101" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q101" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A102" s="23"/>
       <c r="B102" s="24"/>
       <c r="C102" s="25"/>
@@ -4257,19 +4265,19 @@
       <c r="G102" s="26"/>
       <c r="H102" s="27"/>
       <c r="I102" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K102" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q102" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:18" s="3" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>22</v>
       </c>
@@ -4293,20 +4301,20 @@
       </c>
       <c r="H103" s="36"/>
       <c r="I103" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J103" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K103" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q103" s="2">
         <v>28</v>
       </c>
       <c r="R103" s="2"/>
     </row>
-    <row r="104" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A104" s="23">
         <v>23</v>
       </c>
@@ -4330,19 +4338,19 @@
       </c>
       <c r="H104" s="27"/>
       <c r="I104" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J104" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K104" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q104" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A105" s="23"/>
       <c r="B105" s="24"/>
       <c r="C105" s="25"/>
@@ -4352,19 +4360,19 @@
       <c r="G105" s="26"/>
       <c r="H105" s="27"/>
       <c r="I105" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J105" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K105" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q105" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>24</v>
       </c>
@@ -4388,19 +4396,19 @@
       </c>
       <c r="H106" s="36"/>
       <c r="I106" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J106" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K106" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q106" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A107" s="23">
         <v>26</v>
       </c>
@@ -4424,19 +4432,19 @@
       </c>
       <c r="H107" s="27"/>
       <c r="I107" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J107" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K107" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q107" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A108" s="23"/>
       <c r="B108" s="24"/>
       <c r="C108" s="25"/>
@@ -4446,19 +4454,19 @@
       <c r="G108" s="26"/>
       <c r="H108" s="27"/>
       <c r="I108" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J108" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K108" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q108" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A109" s="23"/>
       <c r="B109" s="24"/>
       <c r="C109" s="25"/>
@@ -4468,19 +4476,19 @@
       <c r="G109" s="26"/>
       <c r="H109" s="27"/>
       <c r="I109" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J109" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K109" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q109" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:18" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>27</v>
       </c>
@@ -4503,19 +4511,19 @@
         <v>0.15875</v>
       </c>
       <c r="I110" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J110" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K110" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q110" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A111" s="23">
         <v>28</v>
       </c>
@@ -4539,19 +4547,19 @@
       </c>
       <c r="H111" s="27"/>
       <c r="I111" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J111" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K111" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q111" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A112" s="23"/>
       <c r="B112" s="24"/>
       <c r="C112" s="25"/>
@@ -4561,80 +4569,80 @@
       <c r="G112" s="26"/>
       <c r="H112" s="27"/>
       <c r="I112" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J112" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K112" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q112" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A113" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B113" s="61"/>
-      <c r="C113" s="61"/>
-      <c r="D113" s="61"/>
-      <c r="E113" s="61"/>
-      <c r="F113" s="61"/>
-      <c r="G113" s="61"/>
-      <c r="H113" s="61"/>
-      <c r="I113" s="61"/>
-      <c r="J113" s="61"/>
-      <c r="K113" s="61"/>
-    </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C114" s="62" t="s">
+    <row r="113" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A113" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="B113" s="62"/>
+      <c r="C113" s="62"/>
+      <c r="D113" s="62"/>
+      <c r="E113" s="62"/>
+      <c r="F113" s="62"/>
+      <c r="G113" s="62"/>
+      <c r="H113" s="62"/>
+      <c r="I113" s="62"/>
+      <c r="J113" s="62"/>
+      <c r="K113" s="62"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C114" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D114" s="63"/>
+      <c r="E114" s="29"/>
+      <c r="F114" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D114" s="62"/>
-      <c r="E114" s="29"/>
-      <c r="F114" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G114" s="62"/>
-    </row>
-    <row r="115" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G114" s="63"/>
+    </row>
+    <row r="115" spans="1:18" ht="26" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D115" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E115" s="4"/>
       <c r="F115" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G115" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H115" s="31"/>
       <c r="I115" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K115" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q115" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R115" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="116" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A116" s="23">
         <v>30</v>
       </c>
@@ -4658,19 +4666,19 @@
       </c>
       <c r="H116" s="27"/>
       <c r="I116" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J116" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K116" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q116" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="117" spans="1:18" s="58" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" s="58" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A117" s="23"/>
       <c r="B117" s="24"/>
       <c r="C117" s="25"/>
@@ -4683,16 +4691,16 @@
         <v>1</v>
       </c>
       <c r="J117" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K117" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q117" s="58">
         <v>36</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>32</v>
       </c>
@@ -4716,19 +4724,19 @@
       </c>
       <c r="H118" s="36"/>
       <c r="I118" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J118" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K118" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q118" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A119" s="3"/>
       <c r="B119" s="33"/>
       <c r="C119" s="34"/>
@@ -4738,19 +4746,19 @@
       <c r="G119" s="35"/>
       <c r="H119" s="36"/>
       <c r="I119" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J119" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K119" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q119" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A120" s="23">
         <v>33</v>
       </c>
@@ -4774,19 +4782,19 @@
       </c>
       <c r="H120" s="27"/>
       <c r="I120" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J120" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K120" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q120" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A121" s="23"/>
       <c r="B121" s="24"/>
       <c r="C121" s="25"/>
@@ -4796,19 +4804,19 @@
       <c r="G121" s="26"/>
       <c r="H121" s="27"/>
       <c r="I121" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K121" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q121" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>35</v>
       </c>
@@ -4831,33 +4839,33 @@
         <v>2.30499999999999E-2</v>
       </c>
       <c r="I122" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J122" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K122" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q122" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I123" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J123" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K123" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q123" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A124" s="23">
         <v>43</v>
       </c>
@@ -4881,19 +4889,19 @@
       </c>
       <c r="H124" s="27"/>
       <c r="I124" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J124" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K124" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q124" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A125" s="23"/>
       <c r="B125" s="24"/>
       <c r="C125" s="25"/>
@@ -4903,19 +4911,19 @@
       <c r="G125" s="26"/>
       <c r="H125" s="27"/>
       <c r="I125" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K125" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q125" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>46</v>
       </c>
@@ -4939,19 +4947,19 @@
       </c>
       <c r="H126" s="36"/>
       <c r="I126" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J126" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K126" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q126" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A127" s="3"/>
       <c r="B127" s="33"/>
       <c r="C127" s="34"/>
@@ -4961,19 +4969,19 @@
       <c r="G127" s="35"/>
       <c r="H127" s="36"/>
       <c r="I127" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J127" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K127" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q127" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A128" s="3"/>
       <c r="B128" s="33"/>
       <c r="C128" s="34"/>
@@ -4983,19 +4991,19 @@
       <c r="G128" s="35"/>
       <c r="H128" s="36"/>
       <c r="I128" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J128" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K128" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q128" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A129" s="23">
         <v>49</v>
       </c>
@@ -5025,7 +5033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="130" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>50</v>
       </c>
@@ -5049,19 +5057,19 @@
       </c>
       <c r="H130" s="36"/>
       <c r="I130" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J130" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K130" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q130" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A131" s="40"/>
       <c r="B131" s="41"/>
       <c r="C131" s="42"/>
@@ -5071,19 +5079,19 @@
       <c r="G131" s="43"/>
       <c r="H131" s="44"/>
       <c r="I131" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J131" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K131" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q131" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A132" s="40"/>
       <c r="B132" s="41"/>
       <c r="C132" s="42"/>
@@ -5096,68 +5104,68 @@
       <c r="J132" s="19"/>
       <c r="K132" s="19"/>
     </row>
-    <row r="133" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B133" s="61"/>
-      <c r="C133" s="61"/>
-      <c r="D133" s="61"/>
-      <c r="E133" s="61"/>
-      <c r="F133" s="61"/>
-      <c r="G133" s="61"/>
-      <c r="H133" s="61"/>
-      <c r="I133" s="61"/>
-      <c r="J133" s="61"/>
-      <c r="K133" s="61"/>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C134" s="62" t="s">
+    <row r="133" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A133" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="B133" s="62"/>
+      <c r="C133" s="62"/>
+      <c r="D133" s="62"/>
+      <c r="E133" s="62"/>
+      <c r="F133" s="62"/>
+      <c r="G133" s="62"/>
+      <c r="H133" s="62"/>
+      <c r="I133" s="62"/>
+      <c r="J133" s="62"/>
+      <c r="K133" s="62"/>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C134" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D134" s="63"/>
+      <c r="E134" s="29"/>
+      <c r="F134" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D134" s="62"/>
-      <c r="E134" s="29"/>
-      <c r="F134" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G134" s="62"/>
-    </row>
-    <row r="135" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G134" s="63"/>
+    </row>
+    <row r="135" spans="1:18" ht="26" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B135" s="4"/>
       <c r="C135" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D135" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E135" s="4"/>
       <c r="F135" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G135" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H135" s="31"/>
       <c r="I135" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J135" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K135" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q135" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R135" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="136" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A136" s="50">
         <v>51</v>
       </c>
@@ -5181,19 +5189,19 @@
       </c>
       <c r="H136" s="54"/>
       <c r="I136" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J136" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K136" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q136" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>52</v>
       </c>
@@ -5217,19 +5225,19 @@
       </c>
       <c r="H137" s="36"/>
       <c r="I137" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J137" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K137" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q137" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A138" s="3"/>
       <c r="B138" s="33"/>
       <c r="C138" s="34"/>
@@ -5239,17 +5247,17 @@
       <c r="G138" s="35"/>
       <c r="H138" s="36"/>
       <c r="I138" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J138" s="8"/>
       <c r="K138" s="60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q138" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A139" s="3"/>
       <c r="B139" s="33"/>
       <c r="C139" s="34"/>
@@ -5259,19 +5267,19 @@
       <c r="G139" s="35"/>
       <c r="H139" s="36"/>
       <c r="I139" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J139" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K139" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q139" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A140" s="3"/>
       <c r="B140" s="33"/>
       <c r="C140" s="34"/>
@@ -5281,19 +5289,19 @@
       <c r="G140" s="35"/>
       <c r="H140" s="36"/>
       <c r="I140" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J140" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K140" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q140" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="141" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A141" s="23">
         <v>54</v>
       </c>
@@ -5317,19 +5325,19 @@
       </c>
       <c r="H141" s="27"/>
       <c r="I141" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J141" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K141" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q141" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="142" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A142" s="23"/>
       <c r="B142" s="24"/>
       <c r="C142" s="25"/>
@@ -5339,19 +5347,19 @@
       <c r="G142" s="26"/>
       <c r="H142" s="27"/>
       <c r="I142" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J142" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K142" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q142" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>55</v>
       </c>
@@ -5374,19 +5382,19 @@
         <v>5.4750000000000198E-3</v>
       </c>
       <c r="I143" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J143" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K143" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q143" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A144" s="23">
         <v>57</v>
       </c>
@@ -5410,19 +5418,19 @@
       </c>
       <c r="H144" s="27"/>
       <c r="I144" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J144" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K144" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q144" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="145" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>58</v>
       </c>
@@ -5446,19 +5454,19 @@
       </c>
       <c r="H145" s="36"/>
       <c r="I145" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J145" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K145" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q145" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A146" s="23">
         <v>59</v>
       </c>
@@ -5482,19 +5490,19 @@
       </c>
       <c r="H146" s="27"/>
       <c r="I146" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J146" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K146" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q146" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="147" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>62</v>
       </c>
@@ -5518,19 +5526,19 @@
       </c>
       <c r="H147" s="36"/>
       <c r="I147" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J147" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K147" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q147" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="148" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A148" s="23">
         <v>67</v>
       </c>
@@ -5554,19 +5562,19 @@
       </c>
       <c r="H148" s="27"/>
       <c r="I148" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J148" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K148" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q148" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="149" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>68</v>
       </c>
@@ -5590,19 +5598,19 @@
       </c>
       <c r="H149" s="36"/>
       <c r="I149" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J149" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K149" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q149" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="150" spans="1:18" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A150" s="3"/>
       <c r="B150" s="33"/>
       <c r="C150" s="34"/>
@@ -5612,19 +5620,19 @@
       <c r="G150" s="35"/>
       <c r="H150" s="36"/>
       <c r="I150" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J150" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K150" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q150" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="151" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A151" s="3"/>
       <c r="B151" s="33"/>
       <c r="C151" s="34"/>
@@ -5634,19 +5642,19 @@
       <c r="G151" s="35"/>
       <c r="H151" s="36"/>
       <c r="I151" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J151" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K151" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q151" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="152" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A152" s="3"/>
       <c r="B152" s="33"/>
       <c r="C152" s="34"/>
@@ -5659,7 +5667,7 @@
       <c r="J152" s="18"/>
       <c r="K152" s="8"/>
     </row>
-    <row r="153" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A153" s="3"/>
       <c r="B153" s="33"/>
       <c r="C153" s="34"/>
@@ -5672,7 +5680,7 @@
       <c r="J153" s="18"/>
       <c r="K153" s="8"/>
     </row>
-    <row r="154" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A154" s="3"/>
       <c r="B154" s="33"/>
       <c r="C154" s="34"/>
@@ -5685,68 +5693,68 @@
       <c r="J154" s="18"/>
       <c r="K154" s="8"/>
     </row>
-    <row r="155" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B155" s="61"/>
-      <c r="C155" s="61"/>
-      <c r="D155" s="61"/>
-      <c r="E155" s="61"/>
-      <c r="F155" s="61"/>
-      <c r="G155" s="61"/>
-      <c r="H155" s="61"/>
-      <c r="I155" s="61"/>
-      <c r="J155" s="61"/>
-      <c r="K155" s="61"/>
-    </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C156" s="62" t="s">
+    <row r="155" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="B155" s="62"/>
+      <c r="C155" s="62"/>
+      <c r="D155" s="62"/>
+      <c r="E155" s="62"/>
+      <c r="F155" s="62"/>
+      <c r="G155" s="62"/>
+      <c r="H155" s="62"/>
+      <c r="I155" s="62"/>
+      <c r="J155" s="62"/>
+      <c r="K155" s="62"/>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C156" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D156" s="63"/>
+      <c r="E156" s="29"/>
+      <c r="F156" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D156" s="62"/>
-      <c r="E156" s="29"/>
-      <c r="F156" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="G156" s="62"/>
-    </row>
-    <row r="157" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G156" s="63"/>
+    </row>
+    <row r="157" spans="1:18" ht="26" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B157" s="4"/>
       <c r="C157" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D157" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E157" s="4"/>
       <c r="F157" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G157" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H157" s="31"/>
       <c r="I157" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J157" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K157" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q157" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R157" s="32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="158" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A158" s="23">
         <v>69</v>
       </c>
@@ -5770,19 +5778,19 @@
       </c>
       <c r="H158" s="27"/>
       <c r="I158" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J158" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K158" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q158" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="159" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A159" s="50"/>
       <c r="B159" s="51"/>
       <c r="C159" s="52"/>
@@ -5792,19 +5800,19 @@
       <c r="G159" s="53"/>
       <c r="H159" s="54"/>
       <c r="I159" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J159" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K159" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q159" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="160" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A160" s="40">
         <v>74</v>
       </c>
@@ -5828,19 +5836,19 @@
       </c>
       <c r="H160" s="44"/>
       <c r="I160" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J160" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K160" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q160" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A161" s="3"/>
       <c r="B161" s="33"/>
       <c r="C161" s="34"/>
@@ -5850,19 +5858,19 @@
       <c r="G161" s="35"/>
       <c r="H161" s="36"/>
       <c r="I161" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J161" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K161" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q161" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A162" s="23">
         <v>75</v>
       </c>
@@ -5886,19 +5894,19 @@
       </c>
       <c r="H162" s="27"/>
       <c r="I162" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J162" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K162" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q162" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A163" s="23"/>
       <c r="B163" s="24"/>
       <c r="C163" s="25"/>
@@ -5908,19 +5916,19 @@
       <c r="G163" s="26"/>
       <c r="H163" s="27"/>
       <c r="I163" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J163" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K163" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q163" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A164" s="2">
         <v>77</v>
       </c>
@@ -5943,47 +5951,47 @@
         <v>8.4250000000000002E-3</v>
       </c>
       <c r="I164" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J164" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K164" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q164" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="I165" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J165" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K165" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q165" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="166" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="I166" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J166" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K166" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q166" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A167" s="23">
         <v>79</v>
       </c>
@@ -6013,7 +6021,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="168" spans="1:17" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A168" s="3">
         <v>80</v>
       </c>
@@ -6037,19 +6045,19 @@
       </c>
       <c r="H168" s="36"/>
       <c r="I168" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J168" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K168" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q168" s="2">
         <v>98</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A169" s="23">
         <v>81</v>
       </c>
@@ -6073,19 +6081,19 @@
       </c>
       <c r="H169" s="27"/>
       <c r="I169" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J169" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K169" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q169" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A170" s="2">
         <v>83</v>
       </c>
@@ -6108,30 +6116,30 @@
         <v>6.6499999999999797E-3</v>
       </c>
       <c r="I170" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J170" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K170" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q170" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="I171" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J171" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K171" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="172" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A172" s="23">
         <v>84</v>
       </c>
@@ -6155,19 +6163,19 @@
       </c>
       <c r="H172" s="27"/>
       <c r="I172" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J172" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K172" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q172" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A173" s="23"/>
       <c r="B173" s="24"/>
       <c r="C173" s="25"/>
@@ -6177,17 +6185,17 @@
       <c r="G173" s="26"/>
       <c r="H173" s="27"/>
       <c r="I173" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J173" s="9"/>
       <c r="K173" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q173" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A174" s="2">
         <v>85</v>
       </c>
@@ -6210,19 +6218,19 @@
         <v>6.02499999999998E-3</v>
       </c>
       <c r="I174" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J174" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K174" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q174" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="175" spans="1:17" ht="27" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" ht="23" x14ac:dyDescent="0.35">
       <c r="A175" s="15"/>
       <c r="B175" s="39"/>
       <c r="C175" s="55"/>
@@ -6232,13 +6240,13 @@
       <c r="G175" s="56"/>
       <c r="H175" s="57"/>
       <c r="I175" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J175" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K175" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q175" s="2">
         <v>106</v>
@@ -6246,6 +6254,20 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A155:K155"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="F156:G156"/>
+    <mergeCell ref="A113:K113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="F114:G114"/>
+    <mergeCell ref="A133:K133"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="F134:G134"/>
+    <mergeCell ref="A94:K94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="F95:G95"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="F74:G74"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A22:K22"/>
     <mergeCell ref="A73:K73"/>
@@ -6256,20 +6278,6 @@
     <mergeCell ref="A46:K46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="F47:G47"/>
-    <mergeCell ref="A94:K94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="F95:G95"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="A155:K155"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="F156:G156"/>
-    <mergeCell ref="A113:K113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="F114:G114"/>
-    <mergeCell ref="A133:K133"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="F134:G134"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -6284,104 +6292,104 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" customWidth="1"/>
+    <col min="3" max="3" width="50.453125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="15"/>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="26" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12" t="s">
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="12" t="s">
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="12" t="s">
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="C13" s="16" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working through anonymized texts
</commit_message>
<xml_diff>
--- a/results/dataout_print.xlsx
+++ b/results/dataout_print.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6885" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6890" windowHeight="4730"/>
   </bookViews>
   <sheets>
     <sheet name="dataout" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="128">
   <si>
     <t>Sources of Variability</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Recoded 'incomplete primary' and 'primary complete' as 'secondary'</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>'Self-employed' recoded to zero if 'not in LF' or 'unemployed' scored for employment</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>u_teamid</t>
   </si>
   <si>
-    <t>Part of the data cleaning code not provided</t>
-  </si>
-  <si>
     <t>Country treated as a variance component rather than a dummy</t>
   </si>
   <si>
@@ -343,12 +337,6 @@
     <t>Income variable not recoded, cannot guess how they would have recoded it</t>
   </si>
   <si>
-    <t>Control variable local not defined in submitted code, appears that year dummies were left out</t>
-  </si>
-  <si>
-    <t>Mistakes</t>
-  </si>
-  <si>
     <t>Counter-factual?</t>
   </si>
   <si>
@@ -370,28 +358,16 @@
     <t>Merging process resulting in only 12 countries, mislabeled and introduction of 6,000 extra cases. Curation would require writing nearly new code.</t>
   </si>
   <si>
-    <t>Mistake / lack of adequate skills</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mistake  </t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>Major mistake / procedural</t>
   </si>
   <si>
     <t>Analyzed the two waves of data (1996 &amp; 2006) separately, results are an average</t>
   </si>
   <si>
-    <t>Analyzed the two waves of data (1996 &amp; 2006) separately, results are take as the average</t>
-  </si>
-  <si>
     <t>Mistake / procedural</t>
-  </si>
-  <si>
-    <t xml:space="preserve">After several reviews, code should produce identical results, but regressions contain about 4 thousand less cases. Summary statistics are check and identical with original study. Analysis code from team 56 also produces a 100% exact verification when run on the original study's dataframe. </t>
   </si>
   <si>
     <r>
@@ -425,12 +401,27 @@
   <si>
     <t>Mistake (they specifically stated in their notes that the original study did not mention this, but it was in the code)</t>
   </si>
+  <si>
+    <t>Control variable local not defined in submitted code, year dummies were left out</t>
+  </si>
+  <si>
+    <t>Coded cases as missing rather than 0 when constructing dichotomous variables resulting in roughly 4k less cases in the analyzed data</t>
+  </si>
+  <si>
+    <t>Listwise deletion on all analytical variables</t>
+  </si>
+  <si>
+    <t>Analyzed the two waves of data (1996 &amp; 2006) separately, results are taken as the average</t>
+  </si>
+  <si>
+    <t>Parts of code missing</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,13 +592,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -968,7 +952,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1147,16 +1131,13 @@
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1480,97 +1461,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S176"/>
+  <dimension ref="A1:S177"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I151" sqref="I151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="38" customWidth="1"/>
-    <col min="5" max="6" width="7.5703125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="38" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="30" customWidth="1"/>
-    <col min="9" max="9" width="46.85546875" style="2" customWidth="1"/>
-    <col min="10" max="11" width="15.28515625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="3.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" style="37" customWidth="1"/>
+    <col min="4" max="4" width="7.54296875" style="38" customWidth="1"/>
+    <col min="5" max="6" width="7.54296875" style="37" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" style="38" customWidth="1"/>
+    <col min="8" max="8" width="2.26953125" style="30" customWidth="1"/>
+    <col min="9" max="9" width="46.81640625" style="2" customWidth="1"/>
+    <col min="10" max="11" width="15.26953125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C2" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="62"/>
       <c r="E2" s="29"/>
       <c r="F2" s="62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" s="62"/>
     </row>
-    <row r="3" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D3" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="G3" s="31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="R3" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1604,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="23">
         <v>3</v>
       </c>
@@ -1638,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>9</v>
       </c>
@@ -1671,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="46.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23">
         <v>10</v>
       </c>
@@ -1695,14 +1676,14 @@
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R7" s="2">
         <v>12</v>
@@ -1711,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="97.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="97.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23"/>
       <c r="B8" s="24"/>
       <c r="C8" s="25"/>
@@ -1721,17 +1702,17 @@
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
       <c r="I8" s="7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>15</v>
       </c>
@@ -1764,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="23">
         <v>16</v>
       </c>
@@ -1798,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="34.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>17</v>
       </c>
@@ -1821,14 +1802,14 @@
         <v>3.2916666666666498E-3</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R11" s="2">
         <v>21</v>
@@ -1837,7 +1818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="23">
         <v>19</v>
       </c>
@@ -1871,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>21</v>
       </c>
@@ -1904,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="23">
         <v>25</v>
       </c>
@@ -1931,11 +1912,11 @@
         <v>23</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R14" s="2">
         <v>31</v>
@@ -1944,7 +1925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="23"/>
       <c r="B15" s="24"/>
       <c r="C15" s="25"/>
@@ -1957,11 +1938,11 @@
         <v>24</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R15" s="2">
         <v>31</v>
@@ -1970,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A16" s="23"/>
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
@@ -1980,14 +1961,14 @@
       <c r="G16" s="26"/>
       <c r="H16" s="27"/>
       <c r="I16" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R16" s="2">
         <v>31</v>
@@ -1996,7 +1977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>29</v>
       </c>
@@ -2029,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A18" s="23">
         <v>31</v>
       </c>
@@ -2053,14 +2034,14 @@
       </c>
       <c r="H18" s="27"/>
       <c r="I18" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R18" s="2">
         <v>37</v>
@@ -2069,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A19" s="23"/>
       <c r="B19" s="24"/>
       <c r="C19" s="25"/>
@@ -2082,11 +2063,11 @@
         <v>30</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R19" s="2">
         <v>37</v>
@@ -2095,7 +2076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>34</v>
       </c>
@@ -2122,11 +2103,11 @@
         <v>2</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R20" s="2">
         <v>40</v>
@@ -2135,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="23">
         <v>36</v>
       </c>
@@ -2169,70 +2150,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="63"/>
-      <c r="L22" s="63"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C23" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" s="62"/>
       <c r="E23" s="29"/>
       <c r="F23" s="62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G23" s="62"/>
     </row>
-    <row r="24" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H24" s="31"/>
       <c r="I24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="R24" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S24" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>37</v>
       </c>
@@ -2258,11 +2239,11 @@
         <v>3</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R25" s="2">
         <v>43</v>
@@ -2271,16 +2252,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R26" s="2">
         <v>43</v>
@@ -2289,16 +2270,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I27" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R27" s="2">
         <v>43</v>
@@ -2307,16 +2288,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="I28" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R28" s="2">
         <v>43</v>
@@ -2325,14 +2306,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I29" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R29" s="2">
         <v>43</v>
@@ -2341,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="23">
         <v>38</v>
       </c>
@@ -2375,7 +2356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>39</v>
       </c>
@@ -2398,14 +2379,14 @@
         <v>7.1666666666666502E-3</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K31" s="6"/>
       <c r="L31" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R31" s="2">
         <v>46</v>
@@ -2414,16 +2395,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="I32" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K32" s="6"/>
       <c r="L32" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R32" s="2">
         <v>46</v>
@@ -2432,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="23">
         <v>40</v>
       </c>
@@ -2466,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>41</v>
       </c>
@@ -2492,13 +2473,13 @@
         <v>39</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R34" s="2">
         <v>48</v>
@@ -2507,16 +2488,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I35" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K35" s="6"/>
       <c r="L35" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R35" s="2">
         <v>48</v>
@@ -2525,16 +2506,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="I36" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K36" s="6"/>
       <c r="L36" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R36" s="2">
         <v>48</v>
@@ -2543,16 +2524,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="I37" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K37" s="6"/>
       <c r="L37" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R37" s="2">
         <v>48</v>
@@ -2561,17 +2542,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="81" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
       <c r="I38" s="6" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-    </row>
-    <row r="39" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="L38" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="23">
         <v>42</v>
       </c>
@@ -2605,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>44</v>
       </c>
@@ -2639,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A41" s="23">
         <v>45</v>
       </c>
@@ -2663,14 +2646,14 @@
       </c>
       <c r="H41" s="27"/>
       <c r="I41" s="7" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K41" s="7"/>
       <c r="L41" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R41" s="2">
         <v>53</v>
@@ -2679,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:19" s="58" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="58">
         <v>47</v>
       </c>
@@ -2713,7 +2696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>48</v>
       </c>
@@ -2737,14 +2720,14 @@
       </c>
       <c r="H43" s="36"/>
       <c r="I43" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K43" s="8"/>
       <c r="L43" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R43" s="2">
         <v>57</v>
@@ -2753,7 +2736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="33"/>
       <c r="C44" s="34"/>
@@ -2763,14 +2746,14 @@
       <c r="G44" s="35"/>
       <c r="H44" s="36"/>
       <c r="I44" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K44" s="18"/>
       <c r="L44" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R44" s="2">
         <v>57</v>
@@ -2779,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A45" s="23">
         <v>53</v>
       </c>
@@ -2803,14 +2786,14 @@
       </c>
       <c r="H45" s="27"/>
       <c r="I45" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K45" s="7"/>
       <c r="L45" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R45" s="2">
         <v>62</v>
@@ -2819,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="23"/>
       <c r="B46" s="24"/>
       <c r="C46" s="25"/>
@@ -2833,70 +2816,70 @@
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
     </row>
-    <row r="47" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
-      <c r="K47" s="63"/>
-      <c r="L47" s="63"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="60"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="60"/>
+      <c r="L47" s="60"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C48" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D48" s="62"/>
       <c r="E48" s="29"/>
       <c r="F48" s="62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G48" s="62"/>
     </row>
-    <row r="49" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G49" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H49" s="31"/>
       <c r="I49" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="R49" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S49" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" ht="67.5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>56</v>
       </c>
@@ -2920,14 +2903,14 @@
       </c>
       <c r="H50" s="36"/>
       <c r="I50" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R50" s="2">
         <v>67</v>
@@ -2936,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="23">
         <v>60</v>
       </c>
@@ -2960,14 +2943,14 @@
       </c>
       <c r="H51" s="27"/>
       <c r="I51" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K51" s="7"/>
       <c r="L51" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R51" s="2">
         <v>72</v>
@@ -2976,7 +2959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="40">
         <v>61</v>
       </c>
@@ -3010,7 +2993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="23">
         <v>63</v>
       </c>
@@ -3044,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>64</v>
       </c>
@@ -3078,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="23">
         <v>65</v>
       </c>
@@ -3102,14 +3085,14 @@
       </c>
       <c r="H55" s="27"/>
       <c r="I55" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K55" s="7"/>
       <c r="L55" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R55" s="2">
         <v>77</v>
@@ -3118,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>66</v>
       </c>
@@ -3145,11 +3128,11 @@
         <v>1</v>
       </c>
       <c r="J56" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K56" s="8"/>
       <c r="L56" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R56" s="2">
         <v>79</v>
@@ -3158,7 +3141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="33"/>
       <c r="C57" s="34"/>
@@ -3171,11 +3154,11 @@
         <v>2</v>
       </c>
       <c r="J57" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K57" s="8"/>
       <c r="L57" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R57" s="2">
         <v>79</v>
@@ -3184,7 +3167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="33"/>
       <c r="C58" s="34"/>
@@ -3194,14 +3177,14 @@
       <c r="G58" s="35"/>
       <c r="H58" s="36"/>
       <c r="I58" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K58" s="8"/>
       <c r="L58" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R58" s="2">
         <v>79</v>
@@ -3210,7 +3193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="33"/>
       <c r="C59" s="34"/>
@@ -3220,14 +3203,14 @@
       <c r="G59" s="35"/>
       <c r="H59" s="36"/>
       <c r="I59" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J59" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K59" s="8"/>
       <c r="L59" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R59" s="2">
         <v>79</v>
@@ -3236,7 +3219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A60" s="23">
         <v>70</v>
       </c>
@@ -3260,14 +3243,14 @@
       </c>
       <c r="H60" s="27"/>
       <c r="I60" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J60" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K60" s="7"/>
       <c r="L60" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R60" s="2">
         <v>84</v>
@@ -3276,7 +3259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>71</v>
       </c>
@@ -3309,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A62" s="23">
         <v>72</v>
       </c>
@@ -3333,14 +3316,14 @@
       </c>
       <c r="H62" s="27"/>
       <c r="I62" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K62" s="7"/>
       <c r="L62" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R62" s="2">
         <v>87</v>
@@ -3349,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="23"/>
       <c r="B63" s="24"/>
       <c r="C63" s="25"/>
@@ -3359,14 +3342,14 @@
       <c r="G63" s="26"/>
       <c r="H63" s="27"/>
       <c r="I63" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J63" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K63" s="7"/>
       <c r="L63" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R63" s="2">
         <v>87</v>
@@ -3375,7 +3358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:19" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>73</v>
       </c>
@@ -3409,7 +3392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:19" s="3" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="23">
         <v>76</v>
       </c>
@@ -3433,7 +3416,7 @@
       </c>
       <c r="H65" s="27"/>
       <c r="I65" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
@@ -3445,7 +3428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>78</v>
       </c>
@@ -3479,7 +3462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="45">
         <v>82</v>
       </c>
@@ -3513,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="33"/>
       <c r="C68" s="34"/>
@@ -3527,7 +3510,7 @@
       <c r="K68" s="8"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
       <c r="B69" s="33"/>
       <c r="C69" s="34"/>
@@ -3541,7 +3524,7 @@
       <c r="K69" s="8"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="33"/>
       <c r="C70" s="34"/>
@@ -3555,7 +3538,7 @@
       <c r="K70" s="8"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="33"/>
       <c r="C71" s="34"/>
@@ -3569,7 +3552,7 @@
       <c r="K71" s="8"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A72" s="3"/>
       <c r="B72" s="33"/>
       <c r="C72" s="34"/>
@@ -3583,7 +3566,7 @@
       <c r="K72" s="8"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" s="3"/>
       <c r="B73" s="33"/>
       <c r="C73" s="34"/>
@@ -3597,9 +3580,9 @@
       <c r="K73" s="8"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="61" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B74" s="61"/>
       <c r="C74" s="61"/>
@@ -3613,54 +3596,54 @@
       <c r="K74" s="61"/>
       <c r="L74" s="61"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C75" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D75" s="62"/>
       <c r="E75" s="29"/>
       <c r="F75" s="62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G75" s="62"/>
     </row>
-    <row r="76" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D76" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G76" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H76" s="31"/>
       <c r="I76" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K76" s="5"/>
       <c r="L76" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="R76" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S76" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>1</v>
       </c>
@@ -3683,20 +3666,20 @@
         <v>2.37499999999999E-3</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K77" s="6"/>
       <c r="L77" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R77" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" s="23">
         <v>4</v>
       </c>
@@ -3723,17 +3706,17 @@
         <v>1</v>
       </c>
       <c r="J78" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K78" s="7"/>
       <c r="L78" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R78" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A79" s="23"/>
       <c r="B79" s="24"/>
       <c r="C79" s="25"/>
@@ -3743,20 +3726,20 @@
       <c r="G79" s="26"/>
       <c r="H79" s="27"/>
       <c r="I79" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J79" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K79" s="7"/>
       <c r="L79" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R79" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>5</v>
       </c>
@@ -3782,47 +3765,47 @@
         <v>31</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K80" s="6"/>
       <c r="L80" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R80" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I81" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K81" s="6"/>
       <c r="L81" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R81" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I82" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K82" s="6"/>
       <c r="L82" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R82" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A83" s="23">
         <v>6</v>
       </c>
@@ -3846,20 +3829,20 @@
       </c>
       <c r="H83" s="27"/>
       <c r="I83" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J83" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K83" s="7"/>
       <c r="L83" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R83" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A84" s="23"/>
       <c r="B84" s="24"/>
       <c r="C84" s="25"/>
@@ -3869,20 +3852,20 @@
       <c r="G84" s="26"/>
       <c r="H84" s="27"/>
       <c r="I84" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K84" s="7"/>
       <c r="L84" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R84" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>7</v>
       </c>
@@ -3905,35 +3888,35 @@
         <v>3.5297297297297199E-2</v>
       </c>
       <c r="I85" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K85" s="6"/>
       <c r="L85" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R85" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I86" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J86" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K86" s="6"/>
       <c r="L86" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R86" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A87" s="23">
         <v>8</v>
       </c>
@@ -3957,20 +3940,20 @@
       </c>
       <c r="H87" s="27"/>
       <c r="I87" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K87" s="7"/>
       <c r="L87" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R87" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A88" s="23"/>
       <c r="B88" s="24"/>
       <c r="C88" s="25"/>
@@ -3980,20 +3963,20 @@
       <c r="G88" s="26"/>
       <c r="H88" s="27"/>
       <c r="I88" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J88" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K88" s="7"/>
       <c r="L88" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R88" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>11</v>
       </c>
@@ -4016,20 +3999,20 @@
         <v>1.9E-2</v>
       </c>
       <c r="I89" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J89" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K89" s="6"/>
       <c r="L89" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R89" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="23">
         <v>12</v>
       </c>
@@ -4056,17 +4039,17 @@
         <v>13</v>
       </c>
       <c r="J90" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K90" s="7"/>
       <c r="L90" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R90" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A91" s="23"/>
       <c r="B91" s="24"/>
       <c r="C91" s="25"/>
@@ -4076,17 +4059,17 @@
       <c r="G91" s="26"/>
       <c r="H91" s="27"/>
       <c r="I91" s="7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J91" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K91" s="7"/>
       <c r="L91" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A92" s="23"/>
       <c r="B92" s="24"/>
       <c r="C92" s="25"/>
@@ -4096,20 +4079,20 @@
       <c r="G92" s="26"/>
       <c r="H92" s="27"/>
       <c r="I92" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J92" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K92" s="7"/>
       <c r="L92" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R92" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>13</v>
       </c>
@@ -4132,28 +4115,28 @@
         <v>6.4749999999999903E-3</v>
       </c>
       <c r="I93" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J93" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K93" s="8"/>
       <c r="L93" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R93" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I94" s="6"/>
       <c r="J94" s="8"/>
       <c r="K94" s="8"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" s="61" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B95" s="61"/>
       <c r="C95" s="61"/>
@@ -4167,54 +4150,54 @@
       <c r="K95" s="61"/>
       <c r="L95" s="61"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C96" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D96" s="62"/>
       <c r="E96" s="29"/>
       <c r="F96" s="62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G96" s="62"/>
     </row>
-    <row r="97" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D97" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G97" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H97" s="31"/>
       <c r="I97" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K97" s="5"/>
       <c r="L97" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="R97" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S97" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A98" s="23">
         <v>14</v>
       </c>
@@ -4241,17 +4224,17 @@
         <v>20</v>
       </c>
       <c r="J98" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K98" s="7"/>
       <c r="L98" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R98" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>18</v>
       </c>
@@ -4275,20 +4258,20 @@
       </c>
       <c r="H99" s="36"/>
       <c r="I99" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J99" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K99" s="8"/>
       <c r="L99" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R99" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A100" s="3"/>
       <c r="B100" s="33"/>
       <c r="C100" s="34"/>
@@ -4298,20 +4281,20 @@
       <c r="G100" s="35"/>
       <c r="H100" s="36"/>
       <c r="I100" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J100" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K100" s="8"/>
       <c r="L100" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R100" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A101" s="23">
         <v>20</v>
       </c>
@@ -4338,17 +4321,17 @@
         <v>1</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K101" s="7"/>
       <c r="L101" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R101" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A102" s="50"/>
       <c r="B102" s="51"/>
       <c r="C102" s="52"/>
@@ -4358,20 +4341,20 @@
       <c r="G102" s="53"/>
       <c r="H102" s="54"/>
       <c r="I102" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K102" s="7"/>
       <c r="L102" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R102" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A103" s="23"/>
       <c r="B103" s="24"/>
       <c r="C103" s="25"/>
@@ -4381,20 +4364,20 @@
       <c r="G103" s="26"/>
       <c r="H103" s="27"/>
       <c r="I103" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K103" s="7"/>
       <c r="L103" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R103" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="1:19" s="3" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>22</v>
       </c>
@@ -4421,18 +4404,18 @@
         <v>22</v>
       </c>
       <c r="J104" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K104" s="8"/>
       <c r="L104" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R104" s="2">
         <v>28</v>
       </c>
       <c r="S104" s="2"/>
     </row>
-    <row r="105" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A105" s="23">
         <v>23</v>
       </c>
@@ -4456,20 +4439,20 @@
       </c>
       <c r="H105" s="27"/>
       <c r="I105" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J105" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K105" s="7"/>
       <c r="L105" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R105" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A106" s="23"/>
       <c r="B106" s="24"/>
       <c r="C106" s="25"/>
@@ -4479,20 +4462,20 @@
       <c r="G106" s="26"/>
       <c r="H106" s="27"/>
       <c r="I106" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J106" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K106" s="7"/>
       <c r="L106" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R106" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>24</v>
       </c>
@@ -4516,20 +4499,20 @@
       </c>
       <c r="H107" s="36"/>
       <c r="I107" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J107" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K107" s="8"/>
       <c r="L107" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R107" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A108" s="23">
         <v>26</v>
       </c>
@@ -4556,17 +4539,17 @@
         <v>25</v>
       </c>
       <c r="J108" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K108" s="7"/>
       <c r="L108" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R108" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A109" s="23"/>
       <c r="B109" s="24"/>
       <c r="C109" s="25"/>
@@ -4579,17 +4562,17 @@
         <v>26</v>
       </c>
       <c r="J109" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K109" s="7"/>
       <c r="L109" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R109" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A110" s="23"/>
       <c r="B110" s="24"/>
       <c r="C110" s="25"/>
@@ -4599,20 +4582,20 @@
       <c r="G110" s="26"/>
       <c r="H110" s="27"/>
       <c r="I110" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J110" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K110" s="7"/>
       <c r="L110" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R110" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>27</v>
       </c>
@@ -4638,19 +4621,19 @@
         <v>27</v>
       </c>
       <c r="J111" s="8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K111" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L111" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R111" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A112" s="23">
         <v>28</v>
       </c>
@@ -4677,17 +4660,17 @@
         <v>28</v>
       </c>
       <c r="J112" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K112" s="7"/>
       <c r="L112" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R112" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A113" s="23"/>
       <c r="B113" s="24"/>
       <c r="C113" s="25"/>
@@ -4700,19 +4683,19 @@
         <v>29</v>
       </c>
       <c r="J113" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="K113" s="7"/>
       <c r="L113" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R113" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A114" s="61" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B114" s="61"/>
       <c r="C114" s="61"/>
@@ -4726,54 +4709,54 @@
       <c r="K114" s="61"/>
       <c r="L114" s="61"/>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C115" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D115" s="62"/>
       <c r="E115" s="29"/>
       <c r="F115" s="62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G115" s="62"/>
     </row>
-    <row r="116" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D116" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G116" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H116" s="31"/>
       <c r="I116" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J116" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K116" s="5"/>
       <c r="L116" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="R116" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S116" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="117" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A117" s="23">
         <v>30</v>
       </c>
@@ -4797,20 +4780,20 @@
       </c>
       <c r="H117" s="27"/>
       <c r="I117" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J117" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K117" s="7"/>
       <c r="L117" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R117" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="118" spans="1:19" s="58" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" s="58" customFormat="1" ht="23" x14ac:dyDescent="0.35">
       <c r="A118" s="23"/>
       <c r="B118" s="24"/>
       <c r="C118" s="25"/>
@@ -4823,17 +4806,17 @@
         <v>1</v>
       </c>
       <c r="J118" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K118" s="7"/>
       <c r="L118" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R118" s="58">
         <v>36</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>32</v>
       </c>
@@ -4857,20 +4840,20 @@
       </c>
       <c r="H119" s="36"/>
       <c r="I119" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J119" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K119" s="8"/>
       <c r="L119" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R119" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A120" s="3"/>
       <c r="B120" s="33"/>
       <c r="C120" s="34"/>
@@ -4883,17 +4866,17 @@
         <v>29</v>
       </c>
       <c r="J120" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K120" s="8"/>
       <c r="L120" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R120" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A121" s="23">
         <v>33</v>
       </c>
@@ -4917,20 +4900,20 @@
       </c>
       <c r="H121" s="27"/>
       <c r="I121" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K121" s="7"/>
       <c r="L121" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R121" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A122" s="23"/>
       <c r="B122" s="24"/>
       <c r="C122" s="25"/>
@@ -4940,20 +4923,20 @@
       <c r="G122" s="26"/>
       <c r="H122" s="27"/>
       <c r="I122" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J122" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K122" s="7"/>
       <c r="L122" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R122" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>35</v>
       </c>
@@ -4976,35 +4959,35 @@
         <v>2.30499999999999E-2</v>
       </c>
       <c r="I123" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J123" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K123" s="6"/>
       <c r="L123" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R123" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="I124" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J124" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K124" s="6"/>
       <c r="L124" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R124" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A125" s="23">
         <v>43</v>
       </c>
@@ -5031,17 +5014,17 @@
         <v>40</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K125" s="7"/>
       <c r="L125" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R125" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A126" s="23"/>
       <c r="B126" s="24"/>
       <c r="C126" s="25"/>
@@ -5051,20 +5034,20 @@
       <c r="G126" s="26"/>
       <c r="H126" s="27"/>
       <c r="I126" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J126" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K126" s="7"/>
       <c r="L126" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R126" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>46</v>
       </c>
@@ -5088,20 +5071,20 @@
       </c>
       <c r="H127" s="36"/>
       <c r="I127" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J127" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K127" s="8"/>
       <c r="L127" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R127" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A128" s="3"/>
       <c r="B128" s="33"/>
       <c r="C128" s="34"/>
@@ -5111,20 +5094,20 @@
       <c r="G128" s="35"/>
       <c r="H128" s="36"/>
       <c r="I128" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J128" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K128" s="8"/>
       <c r="L128" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R128" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A129" s="3"/>
       <c r="B129" s="33"/>
       <c r="C129" s="34"/>
@@ -5137,17 +5120,17 @@
         <v>29</v>
       </c>
       <c r="J129" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K129" s="8"/>
       <c r="L129" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R129" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130" s="23">
         <v>49</v>
       </c>
@@ -5178,7 +5161,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>50</v>
       </c>
@@ -5202,20 +5185,20 @@
       </c>
       <c r="H131" s="36"/>
       <c r="I131" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J131" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K131" s="8"/>
       <c r="L131" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R131" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A132" s="40"/>
       <c r="B132" s="41"/>
       <c r="C132" s="42"/>
@@ -5225,20 +5208,20 @@
       <c r="G132" s="43"/>
       <c r="H132" s="44"/>
       <c r="I132" s="19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J132" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K132" s="19"/>
       <c r="L132" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R132" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A133" s="40"/>
       <c r="B133" s="41"/>
       <c r="C133" s="42"/>
@@ -5252,9 +5235,9 @@
       <c r="K133" s="19"/>
       <c r="L133" s="19"/>
     </row>
-    <row r="134" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A134" s="61" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B134" s="61"/>
       <c r="C134" s="61"/>
@@ -5268,54 +5251,54 @@
       <c r="K134" s="61"/>
       <c r="L134" s="61"/>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C135" s="62" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D135" s="62"/>
       <c r="E135" s="29"/>
       <c r="F135" s="62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G135" s="62"/>
     </row>
-    <row r="136" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:19" ht="26" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B136" s="4"/>
       <c r="C136" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D136" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E136" s="4"/>
       <c r="F136" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G136" s="31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H136" s="31"/>
       <c r="I136" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J136" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K136" s="5"/>
       <c r="L136" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="R136" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S136" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="137" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A137" s="50">
         <v>51</v>
       </c>
@@ -5339,20 +5322,22 @@
       </c>
       <c r="H137" s="54"/>
       <c r="I137" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J137" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="K137" s="20"/>
+        <v>97</v>
+      </c>
+      <c r="K137" s="20" t="s">
+        <v>95</v>
+      </c>
       <c r="L137" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R137" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>52</v>
       </c>
@@ -5376,20 +5361,20 @@
       </c>
       <c r="H138" s="36"/>
       <c r="I138" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J138" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="K138" s="8"/>
       <c r="L138" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R138" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A139" s="3"/>
       <c r="B139" s="33"/>
       <c r="C139" s="34"/>
@@ -5399,18 +5384,20 @@
       <c r="G139" s="35"/>
       <c r="H139" s="36"/>
       <c r="I139" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="J139" s="8"/>
+        <v>90</v>
+      </c>
+      <c r="J139" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="K139" s="8"/>
-      <c r="L139" s="60" t="s">
-        <v>118</v>
+      <c r="L139" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="R139" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A140" s="3"/>
       <c r="B140" s="33"/>
       <c r="C140" s="34"/>
@@ -5420,20 +5407,20 @@
       <c r="G140" s="35"/>
       <c r="H140" s="36"/>
       <c r="I140" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J140" s="8" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="K140" s="8"/>
       <c r="L140" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R140" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A141" s="3"/>
       <c r="B141" s="33"/>
       <c r="C141" s="34"/>
@@ -5443,20 +5430,20 @@
       <c r="G141" s="35"/>
       <c r="H141" s="36"/>
       <c r="I141" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J141" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K141" s="18"/>
       <c r="L141" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R141" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A142" s="23">
         <v>54</v>
       </c>
@@ -5480,20 +5467,20 @@
       </c>
       <c r="H142" s="27"/>
       <c r="I142" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J142" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K142" s="7"/>
       <c r="L142" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R142" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A143" s="23"/>
       <c r="B143" s="24"/>
       <c r="C143" s="25"/>
@@ -5503,20 +5490,20 @@
       <c r="G143" s="26"/>
       <c r="H143" s="27"/>
       <c r="I143" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J143" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K143" s="7"/>
       <c r="L143" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R143" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>55</v>
       </c>
@@ -5539,20 +5526,20 @@
         <v>5.4750000000000198E-3</v>
       </c>
       <c r="I144" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J144" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K144" s="6"/>
       <c r="L144" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R144" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="27" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A145" s="23">
         <v>57</v>
       </c>
@@ -5576,228 +5563,225 @@
       </c>
       <c r="H145" s="27"/>
       <c r="I145" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J145" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K145" s="7"/>
       <c r="L145" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R145" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="27" x14ac:dyDescent="0.25">
-      <c r="A146" s="3">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A146" s="23"/>
+      <c r="B146" s="24"/>
+      <c r="C146" s="25"/>
+      <c r="D146" s="26"/>
+      <c r="E146" s="25"/>
+      <c r="F146" s="25"/>
+      <c r="G146" s="26"/>
+      <c r="H146" s="27"/>
+      <c r="I146" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="J146" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K146" s="7"/>
+      <c r="L146" s="7"/>
+    </row>
+    <row r="147" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+      <c r="A147" s="3">
         <v>58</v>
       </c>
-      <c r="B146" s="33">
-        <v>1</v>
-      </c>
-      <c r="C146" s="34">
+      <c r="B147" s="33">
+        <v>1</v>
+      </c>
+      <c r="C147" s="34">
         <v>0.8</v>
       </c>
-      <c r="D146" s="35">
+      <c r="D147" s="35">
         <v>6.2999999999999801E-3</v>
       </c>
-      <c r="E146" s="34">
-        <v>1</v>
-      </c>
-      <c r="F146" s="34">
+      <c r="E147" s="34">
+        <v>1</v>
+      </c>
+      <c r="F147" s="34">
         <v>0.8</v>
       </c>
-      <c r="G146" s="35">
+      <c r="G147" s="35">
         <v>6.2999999999999801E-3</v>
       </c>
-      <c r="H146" s="36"/>
-      <c r="I146" s="8" t="s">
+      <c r="H147" s="36"/>
+      <c r="I147" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J147" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K147" s="8"/>
+      <c r="L147" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="R147" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+      <c r="A148" s="23">
+        <v>59</v>
+      </c>
+      <c r="B148" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="C148" s="25">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D148" s="26">
+        <v>0.1275</v>
+      </c>
+      <c r="E148" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="F148" s="25">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G148" s="26">
+        <v>0.1275</v>
+      </c>
+      <c r="H148" s="27"/>
+      <c r="I148" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J148" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K148" s="7"/>
+      <c r="L148" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="R148" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A149" s="3">
+        <v>62</v>
+      </c>
+      <c r="B149" s="33">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="C149" s="34">
+        <v>0.375</v>
+      </c>
+      <c r="D149" s="35">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="E149" s="34">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="F149" s="34">
+        <v>0.375</v>
+      </c>
+      <c r="G149" s="35">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="H149" s="36"/>
+      <c r="I149" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J149" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K149" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="L149" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="R149" s="2">
         <v>74</v>
       </c>
-      <c r="J146" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="K146" s="8"/>
-      <c r="L146" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="R146" s="2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="147" spans="1:19" ht="27" x14ac:dyDescent="0.25">
-      <c r="A147" s="23">
-        <v>59</v>
-      </c>
-      <c r="B147" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="C147" s="25">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="D147" s="26">
-        <v>0.1275</v>
-      </c>
-      <c r="E147" s="25">
-        <v>0.4</v>
-      </c>
-      <c r="F147" s="25">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G147" s="26">
-        <v>0.1275</v>
-      </c>
-      <c r="H147" s="27"/>
-      <c r="I147" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J147" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="K147" s="7"/>
-      <c r="L147" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="R147" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="148" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A148" s="3">
-        <v>62</v>
-      </c>
-      <c r="B148" s="33">
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A150" s="23">
+        <v>67</v>
+      </c>
+      <c r="B150" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="C150" s="25">
+        <v>0</v>
+      </c>
+      <c r="D150" s="26">
+        <v>0.15642500000000001</v>
+      </c>
+      <c r="E150" s="25">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="F150" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="G150" s="26">
+        <v>5.0774999999999897E-2</v>
+      </c>
+      <c r="H150" s="27"/>
+      <c r="I150" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J150" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K150" s="7"/>
+      <c r="L150" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="R150" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+      <c r="A151" s="3">
+        <v>68</v>
+      </c>
+      <c r="B151" s="33">
         <v>0.97499999999999998</v>
       </c>
-      <c r="C148" s="34">
-        <v>0.375</v>
-      </c>
-      <c r="D148" s="35">
-        <v>2.1600000000000001E-2</v>
-      </c>
-      <c r="E148" s="34">
+      <c r="C151" s="34">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="D151" s="35">
+        <v>2.1524999999999999E-2</v>
+      </c>
+      <c r="E151" s="34">
         <v>0.97499999999999998</v>
       </c>
-      <c r="F148" s="34">
-        <v>0.375</v>
-      </c>
-      <c r="G148" s="35">
-        <v>2.1600000000000001E-2</v>
-      </c>
-      <c r="H148" s="36"/>
-      <c r="I148" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J148" s="8" t="s">
+      <c r="F151" s="34">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="G151" s="35">
+        <v>2.1524999999999999E-2</v>
+      </c>
+      <c r="H151" s="36"/>
+      <c r="I151" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J151" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="K148" s="8"/>
-      <c r="L148" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="R148" s="2">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="149" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A149" s="23">
-        <v>67</v>
-      </c>
-      <c r="B149" s="24">
-        <v>0.6</v>
-      </c>
-      <c r="C149" s="25">
-        <v>0</v>
-      </c>
-      <c r="D149" s="26">
-        <v>0.15642500000000001</v>
-      </c>
-      <c r="E149" s="25">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="F149" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="G149" s="26">
-        <v>5.0774999999999897E-2</v>
-      </c>
-      <c r="H149" s="27"/>
-      <c r="I149" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J149" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="K149" s="7"/>
-      <c r="L149" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="R149" s="2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="150" spans="1:19" ht="27" x14ac:dyDescent="0.25">
-      <c r="A150" s="3">
-        <v>68</v>
-      </c>
-      <c r="B150" s="33">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="C150" s="34">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="D150" s="35">
-        <v>2.1524999999999999E-2</v>
-      </c>
-      <c r="E150" s="34">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="F150" s="34">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="G150" s="35">
-        <v>2.1524999999999999E-2</v>
-      </c>
-      <c r="H150" s="36"/>
-      <c r="I150" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="J150" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="K150" s="8"/>
-      <c r="L150" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="R150" s="2">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="151" spans="1:19" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A151" s="3"/>
-      <c r="B151" s="33"/>
-      <c r="C151" s="34"/>
-      <c r="D151" s="35"/>
-      <c r="E151" s="34"/>
-      <c r="F151" s="34"/>
-      <c r="G151" s="35"/>
-      <c r="H151" s="36"/>
-      <c r="I151" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="J151" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="K151" s="18"/>
+      <c r="K151" s="8"/>
       <c r="L151" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R151" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A152" s="3"/>
       <c r="B152" s="33"/>
       <c r="C152" s="34"/>
@@ -5807,20 +5791,20 @@
       <c r="G152" s="35"/>
       <c r="H152" s="36"/>
       <c r="I152" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J152" s="18" t="s">
         <v>101</v>
       </c>
       <c r="K152" s="18"/>
       <c r="L152" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R152" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A153" s="3"/>
       <c r="B153" s="33"/>
       <c r="C153" s="34"/>
@@ -5829,12 +5813,21 @@
       <c r="F153" s="34"/>
       <c r="G153" s="35"/>
       <c r="H153" s="36"/>
-      <c r="I153" s="18"/>
-      <c r="J153" s="18"/>
+      <c r="I153" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J153" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="K153" s="18"/>
-      <c r="L153" s="8"/>
-    </row>
-    <row r="154" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="L153" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="R153" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A154" s="3"/>
       <c r="B154" s="33"/>
       <c r="C154" s="34"/>
@@ -5848,7 +5841,7 @@
       <c r="K154" s="18"/>
       <c r="L154" s="8"/>
     </row>
-    <row r="155" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A155" s="3"/>
       <c r="B155" s="33"/>
       <c r="C155" s="34"/>
@@ -5862,587 +5855,615 @@
       <c r="K155" s="18"/>
       <c r="L155" s="8"/>
     </row>
-    <row r="156" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A156" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="B156" s="61"/>
-      <c r="C156" s="61"/>
-      <c r="D156" s="61"/>
-      <c r="E156" s="61"/>
-      <c r="F156" s="61"/>
-      <c r="G156" s="61"/>
-      <c r="H156" s="61"/>
-      <c r="I156" s="61"/>
-      <c r="J156" s="61"/>
-      <c r="K156" s="61"/>
-      <c r="L156" s="61"/>
-    </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C157" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="D157" s="62"/>
-      <c r="E157" s="29"/>
-      <c r="F157" s="62" t="s">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A156" s="3"/>
+      <c r="B156" s="33"/>
+      <c r="C156" s="34"/>
+      <c r="D156" s="35"/>
+      <c r="E156" s="34"/>
+      <c r="F156" s="34"/>
+      <c r="G156" s="35"/>
+      <c r="H156" s="36"/>
+      <c r="I156" s="18"/>
+      <c r="J156" s="18"/>
+      <c r="K156" s="18"/>
+      <c r="L156" s="8"/>
+    </row>
+    <row r="157" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A157" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="B157" s="61"/>
+      <c r="C157" s="61"/>
+      <c r="D157" s="61"/>
+      <c r="E157" s="61"/>
+      <c r="F157" s="61"/>
+      <c r="G157" s="61"/>
+      <c r="H157" s="61"/>
+      <c r="I157" s="61"/>
+      <c r="J157" s="61"/>
+      <c r="K157" s="61"/>
+      <c r="L157" s="61"/>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="C158" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="D158" s="62"/>
+      <c r="E158" s="29"/>
+      <c r="F158" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="G158" s="62"/>
+    </row>
+    <row r="159" spans="1:19" ht="26" x14ac:dyDescent="0.3">
+      <c r="A159" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B159" s="4"/>
+      <c r="C159" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G157" s="62"/>
-    </row>
-    <row r="158" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A158" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B158" s="4"/>
-      <c r="C158" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D158" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E158" s="4"/>
-      <c r="F158" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G158" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H158" s="31"/>
-      <c r="I158" s="5" t="s">
+      <c r="D159" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G159" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="H159" s="31"/>
+      <c r="I159" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J158" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K158" s="5"/>
-      <c r="L158" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="R158" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="S158" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="159" spans="1:19" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A159" s="23">
+      <c r="J159" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K159" s="5"/>
+      <c r="L159" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="R159" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="S159" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A160" s="23">
         <v>69</v>
       </c>
-      <c r="B159" s="24">
+      <c r="B160" s="24">
         <v>0.85</v>
       </c>
-      <c r="C159" s="25">
+      <c r="C160" s="25">
         <v>0.17499999999999999</v>
       </c>
-      <c r="D159" s="26">
+      <c r="D160" s="26">
         <v>2.81E-2</v>
       </c>
-      <c r="E159" s="25">
-        <v>1</v>
-      </c>
-      <c r="F159" s="25">
+      <c r="E160" s="25">
+        <v>1</v>
+      </c>
+      <c r="F160" s="25">
         <v>0.95</v>
       </c>
-      <c r="G159" s="26">
+      <c r="G160" s="26">
         <v>3.9749999999999803E-3</v>
       </c>
-      <c r="H159" s="27"/>
-      <c r="I159" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="J159" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="K159" s="7"/>
-      <c r="L159" s="7" t="s">
+      <c r="H160" s="27"/>
+      <c r="I160" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J160" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="R159" s="2">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="160" spans="1:19" ht="27" x14ac:dyDescent="0.25">
-      <c r="A160" s="50"/>
-      <c r="B160" s="51"/>
-      <c r="C160" s="52"/>
-      <c r="D160" s="53"/>
-      <c r="E160" s="52"/>
-      <c r="F160" s="52"/>
-      <c r="G160" s="53"/>
-      <c r="H160" s="54"/>
-      <c r="I160" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="J160" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="K160" s="20"/>
-      <c r="L160" s="20" t="s">
-        <v>100</v>
+      <c r="K160" s="7"/>
+      <c r="L160" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="R160" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="161" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A161" s="40">
+    <row r="161" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A161" s="50"/>
+      <c r="B161" s="51"/>
+      <c r="C161" s="52"/>
+      <c r="D161" s="53"/>
+      <c r="E161" s="52"/>
+      <c r="F161" s="52"/>
+      <c r="G161" s="53"/>
+      <c r="H161" s="54"/>
+      <c r="I161" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="J161" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="K161" s="20"/>
+      <c r="L161" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="R161" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A162" s="40">
         <v>74</v>
       </c>
-      <c r="B161" s="41">
+      <c r="B162" s="41">
         <v>0.85</v>
       </c>
-      <c r="C161" s="42">
+      <c r="C162" s="42">
         <v>0.15</v>
       </c>
-      <c r="D161" s="43">
+      <c r="D162" s="43">
         <v>3.8875E-2</v>
       </c>
-      <c r="E161" s="42">
+      <c r="E162" s="42">
         <v>0.85</v>
       </c>
-      <c r="F161" s="42">
+      <c r="F162" s="42">
         <v>0.15</v>
       </c>
-      <c r="G161" s="43">
+      <c r="G162" s="43">
         <v>3.8875E-2</v>
       </c>
-      <c r="H161" s="44"/>
-      <c r="I161" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J161" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="K161" s="19"/>
-      <c r="L161" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="R161" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="162" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A162" s="3"/>
-      <c r="B162" s="33"/>
-      <c r="C162" s="34"/>
-      <c r="D162" s="35"/>
-      <c r="E162" s="34"/>
-      <c r="F162" s="34"/>
-      <c r="G162" s="35"/>
-      <c r="H162" s="36"/>
-      <c r="I162" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="J162" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="K162" s="8"/>
-      <c r="L162" s="8" t="s">
-        <v>100</v>
+      <c r="H162" s="44"/>
+      <c r="I162" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J162" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K162" s="19"/>
+      <c r="L162" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="R162" s="2">
         <v>90</v>
       </c>
     </row>
-    <row r="163" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A163" s="23">
+    <row r="163" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A163" s="3"/>
+      <c r="B163" s="33"/>
+      <c r="C163" s="34"/>
+      <c r="D163" s="35"/>
+      <c r="E163" s="34"/>
+      <c r="F163" s="34"/>
+      <c r="G163" s="35"/>
+      <c r="H163" s="36"/>
+      <c r="I163" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="J163" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K163" s="8"/>
+      <c r="L163" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="R163" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A164" s="23">
         <v>75</v>
       </c>
-      <c r="B163" s="24">
+      <c r="B164" s="24">
         <v>0.97499999999999998</v>
       </c>
-      <c r="C163" s="25">
+      <c r="C164" s="25">
         <v>0.45</v>
       </c>
-      <c r="D163" s="26">
+      <c r="D164" s="26">
         <v>1.5625E-2</v>
       </c>
-      <c r="E163" s="25">
+      <c r="E164" s="25">
         <v>0.97499999999999998</v>
       </c>
-      <c r="F163" s="25">
+      <c r="F164" s="25">
         <v>0.45</v>
       </c>
-      <c r="G163" s="26">
+      <c r="G164" s="26">
         <v>1.5625E-2</v>
       </c>
-      <c r="H163" s="27"/>
-      <c r="I163" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="J163" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="K163" s="7"/>
-      <c r="L163" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="R163" s="2">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="164" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A164" s="23"/>
-      <c r="B164" s="24"/>
-      <c r="C164" s="25"/>
-      <c r="D164" s="26"/>
-      <c r="E164" s="25"/>
-      <c r="F164" s="25"/>
-      <c r="G164" s="26"/>
       <c r="H164" s="27"/>
       <c r="I164" s="7" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="J164" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K164" s="7"/>
       <c r="L164" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R164" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="165" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A165" s="2">
+    <row r="165" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A165" s="23"/>
+      <c r="B165" s="24"/>
+      <c r="C165" s="25"/>
+      <c r="D165" s="26"/>
+      <c r="E165" s="25"/>
+      <c r="F165" s="25"/>
+      <c r="G165" s="26"/>
+      <c r="H165" s="27"/>
+      <c r="I165" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J165" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K165" s="7"/>
+      <c r="L165" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="R165" s="2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A166" s="2">
         <v>77</v>
       </c>
-      <c r="B165" s="28">
+      <c r="B166" s="28">
         <v>0.72499999999999998</v>
       </c>
-      <c r="C165" s="37">
+      <c r="C166" s="37">
         <v>0</v>
       </c>
-      <c r="D165" s="38">
+      <c r="D166" s="38">
         <v>0.994475</v>
       </c>
-      <c r="E165" s="37">
-        <v>1</v>
-      </c>
-      <c r="F165" s="37">
+      <c r="E166" s="37">
+        <v>1</v>
+      </c>
+      <c r="F166" s="37">
         <v>0.625</v>
       </c>
-      <c r="G165" s="38">
+      <c r="G166" s="38">
         <v>8.4250000000000002E-3</v>
       </c>
-      <c r="I165" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J165" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K165" s="6"/>
-      <c r="L165" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="R165" s="2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="166" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="I166" s="6" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="J166" s="6" t="s">
         <v>103</v>
       </c>
       <c r="K166" s="6"/>
       <c r="L166" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R166" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="167" spans="1:18" ht="27" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" ht="23" x14ac:dyDescent="0.35">
       <c r="I167" s="6" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="J167" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K167" s="6"/>
       <c r="L167" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R167" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="168" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A168" s="23">
+    <row r="168" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="I168" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J168" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K168" s="6"/>
+      <c r="L168" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="R168" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A169" s="23">
         <v>79</v>
       </c>
-      <c r="B168" s="24">
-        <v>1</v>
-      </c>
-      <c r="C168" s="25">
+      <c r="B169" s="24">
+        <v>1</v>
+      </c>
+      <c r="C169" s="25">
         <v>0.95</v>
       </c>
-      <c r="D168" s="26">
+      <c r="D169" s="26">
         <v>2.72499999999999E-3</v>
       </c>
-      <c r="E168" s="25">
-        <v>1</v>
-      </c>
-      <c r="F168" s="25">
+      <c r="E169" s="25">
+        <v>1</v>
+      </c>
+      <c r="F169" s="25">
         <v>0.95</v>
       </c>
-      <c r="G168" s="26">
+      <c r="G169" s="26">
         <v>2.72499999999999E-3</v>
       </c>
-      <c r="H168" s="27"/>
-      <c r="I168" s="7"/>
-      <c r="J168" s="7"/>
-      <c r="K168" s="7"/>
-      <c r="L168" s="7"/>
-      <c r="R168" s="2">
+      <c r="H169" s="27"/>
+      <c r="I169" s="7"/>
+      <c r="J169" s="7"/>
+      <c r="K169" s="7"/>
+      <c r="L169" s="7"/>
+      <c r="R169" s="2">
         <v>97</v>
       </c>
     </row>
-    <row r="169" spans="1:18" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A169" s="3">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A170" s="3">
         <v>80</v>
       </c>
-      <c r="B169" s="33">
+      <c r="B170" s="33">
         <v>0.72499999999999998</v>
       </c>
-      <c r="C169" s="34">
+      <c r="C170" s="34">
         <v>0.05</v>
       </c>
-      <c r="D169" s="35">
+      <c r="D170" s="35">
         <v>0.94814999999999905</v>
       </c>
-      <c r="E169" s="34">
-        <v>1</v>
-      </c>
-      <c r="F169" s="34">
-        <v>1</v>
-      </c>
-      <c r="G169" s="35">
+      <c r="E170" s="34">
+        <v>1</v>
+      </c>
+      <c r="F170" s="34">
+        <v>1</v>
+      </c>
+      <c r="G170" s="35">
         <v>1.89999999999999E-3</v>
       </c>
-      <c r="H169" s="36"/>
-      <c r="I169" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J169" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="K169" s="8"/>
-      <c r="L169" s="8" t="s">
+      <c r="H170" s="36"/>
+      <c r="I170" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J170" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="K170" s="8"/>
+      <c r="L170" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="R170" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A171" s="23">
+        <v>81</v>
+      </c>
+      <c r="B171" s="24">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="C171" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="D171" s="26">
+        <v>0.11877500000000001</v>
+      </c>
+      <c r="E171" s="25">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F171" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="G171" s="26">
+        <v>0.11877500000000001</v>
+      </c>
+      <c r="H171" s="27"/>
+      <c r="I171" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J171" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="R169" s="2">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="170" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A170" s="23">
-        <v>81</v>
-      </c>
-      <c r="B170" s="24">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="C170" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="D170" s="26">
-        <v>0.11877500000000001</v>
-      </c>
-      <c r="E170" s="25">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="F170" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="G170" s="26">
-        <v>0.11877500000000001</v>
-      </c>
-      <c r="H170" s="27"/>
-      <c r="I170" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J170" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="K170" s="7"/>
-      <c r="L170" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="R170" s="2">
+      <c r="K171" s="7"/>
+      <c r="L171" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="R171" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="171" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A171" s="2">
+    <row r="172" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A172" s="2">
         <v>83</v>
       </c>
-      <c r="B171" s="28">
-        <v>1</v>
-      </c>
-      <c r="C171" s="37">
+      <c r="B172" s="28">
+        <v>1</v>
+      </c>
+      <c r="C172" s="37">
         <v>0.72499999999999998</v>
       </c>
-      <c r="D171" s="38">
+      <c r="D172" s="38">
         <v>6.6499999999999797E-3</v>
       </c>
-      <c r="E171" s="37">
-        <v>1</v>
-      </c>
-      <c r="F171" s="37">
+      <c r="E172" s="37">
+        <v>1</v>
+      </c>
+      <c r="F172" s="37">
         <v>0.72499999999999998</v>
       </c>
-      <c r="G171" s="38">
+      <c r="G172" s="38">
         <v>6.6499999999999797E-3</v>
       </c>
-      <c r="I171" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J171" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="K171" s="10"/>
-      <c r="L171" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="R171" s="2">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="172" spans="1:18" ht="27" x14ac:dyDescent="0.25">
       <c r="I172" s="10" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="J172" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K172" s="10"/>
       <c r="L172" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="173" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A173" s="23">
+        <v>98</v>
+      </c>
+      <c r="R172" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="I173" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J173" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K173" s="10"/>
+      <c r="L173" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A174" s="23">
         <v>84</v>
       </c>
-      <c r="B173" s="24">
-        <v>1</v>
-      </c>
-      <c r="C173" s="25">
+      <c r="B174" s="24">
+        <v>1</v>
+      </c>
+      <c r="C174" s="25">
         <v>0.85</v>
       </c>
-      <c r="D173" s="26">
+      <c r="D174" s="26">
         <v>5.37499999999999E-3</v>
       </c>
-      <c r="E173" s="25">
-        <v>1</v>
-      </c>
-      <c r="F173" s="25">
+      <c r="E174" s="25">
+        <v>1</v>
+      </c>
+      <c r="F174" s="25">
         <v>0.85</v>
       </c>
-      <c r="G173" s="26">
+      <c r="G174" s="26">
         <v>5.37499999999999E-3</v>
       </c>
-      <c r="H173" s="27"/>
-      <c r="I173" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J173" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="K173" s="7"/>
-      <c r="L173" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="R173" s="2">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="174" spans="1:18" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A174" s="23"/>
-      <c r="B174" s="24"/>
-      <c r="C174" s="25"/>
-      <c r="D174" s="26"/>
-      <c r="E174" s="25"/>
-      <c r="F174" s="25"/>
-      <c r="G174" s="26"/>
       <c r="H174" s="27"/>
-      <c r="I174" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="J174" s="9"/>
-      <c r="K174" s="9"/>
+      <c r="I174" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J174" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K174" s="7"/>
       <c r="L174" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="R174" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="175" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A175" s="2">
+    <row r="175" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A175" s="23"/>
+      <c r="B175" s="24"/>
+      <c r="C175" s="25"/>
+      <c r="D175" s="26"/>
+      <c r="E175" s="25"/>
+      <c r="F175" s="25"/>
+      <c r="G175" s="26"/>
+      <c r="H175" s="27"/>
+      <c r="I175" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J175" s="9"/>
+      <c r="K175" s="9"/>
+      <c r="L175" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="R175" s="2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A176" s="2">
         <v>85</v>
       </c>
-      <c r="B175" s="28">
-        <v>1</v>
-      </c>
-      <c r="C175" s="37">
+      <c r="B176" s="28">
+        <v>1</v>
+      </c>
+      <c r="C176" s="37">
         <v>0.77500000000000002</v>
       </c>
-      <c r="D175" s="38">
+      <c r="D176" s="38">
         <v>6.02499999999998E-3</v>
       </c>
-      <c r="E175" s="37">
-        <v>1</v>
-      </c>
-      <c r="F175" s="37">
+      <c r="E176" s="37">
+        <v>1</v>
+      </c>
+      <c r="F176" s="37">
         <v>0.77500000000000002</v>
       </c>
-      <c r="G175" s="38">
+      <c r="G176" s="38">
         <v>6.02499999999998E-3</v>
       </c>
-      <c r="I175" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J175" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="K175" s="6"/>
-      <c r="L175" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="R175" s="2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="176" spans="1:18" ht="27" x14ac:dyDescent="0.25">
-      <c r="A176" s="15"/>
-      <c r="B176" s="39"/>
-      <c r="C176" s="55"/>
-      <c r="D176" s="56"/>
-      <c r="E176" s="55"/>
-      <c r="F176" s="55"/>
-      <c r="G176" s="56"/>
-      <c r="H176" s="57"/>
-      <c r="I176" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="J176" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="K176" s="21"/>
-      <c r="L176" s="22" t="s">
-        <v>100</v>
+      <c r="I176" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J176" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K176" s="6"/>
+      <c r="L176" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="R176" s="2">
         <v>106</v>
       </c>
     </row>
+    <row r="177" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+      <c r="A177" s="15"/>
+      <c r="B177" s="39"/>
+      <c r="C177" s="55"/>
+      <c r="D177" s="56"/>
+      <c r="E177" s="55"/>
+      <c r="F177" s="55"/>
+      <c r="G177" s="56"/>
+      <c r="H177" s="57"/>
+      <c r="I177" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="J177" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="K177" s="21"/>
+      <c r="L177" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="R177" s="2">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A157:L157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="F158:G158"/>
+    <mergeCell ref="A114:L114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="F115:G115"/>
+    <mergeCell ref="A134:L134"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="F135:G135"/>
+    <mergeCell ref="A95:L95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="F96:G96"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="F75:G75"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A22:L22"/>
     <mergeCell ref="A74:L74"/>
@@ -6453,20 +6474,6 @@
     <mergeCell ref="A47:L47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="F48:G48"/>
-    <mergeCell ref="A95:L95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="F96:G96"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="A156:L156"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="F157:G157"/>
-    <mergeCell ref="A114:L114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="F115:G115"/>
-    <mergeCell ref="A134:L134"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="F135:G135"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -6481,19 +6488,19 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="5.28515625" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="5.26953125" customWidth="1"/>
+    <col min="3" max="3" width="50.453125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="15"/>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -6501,7 +6508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -6509,7 +6516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="26" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -6517,7 +6524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="26" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -6525,7 +6532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -6533,7 +6540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -6541,7 +6548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
@@ -6549,7 +6556,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
@@ -6557,7 +6564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
@@ -6565,7 +6572,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
@@ -6573,7 +6580,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" s="14" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Table 1 and Table 3 finished
</commit_message>
<xml_diff>
--- a/results/dataout_print.xlsx
+++ b/results/dataout_print.xlsx
@@ -316,9 +316,6 @@
     <t>Interpretational</t>
   </si>
   <si>
-    <t xml:space="preserve">It is not possible to explain seemingly random variation at the third decimal place, even though they used Stata and coding appears identical to original. </t>
-  </si>
-  <si>
     <t>Used a different country as the reference dummy category</t>
   </si>
   <si>
@@ -436,10 +433,13 @@
     <t>Coded as procedural, but exact variation source unknown/unfound by Pis</t>
   </si>
   <si>
-    <t>Coded as procedural, but exact variation source unknown</t>
-  </si>
-  <si>
     <t>Questionable methodological competencies</t>
+  </si>
+  <si>
+    <t>Some variables' values had to be truncated because they were otherwise too precise for MLWin</t>
+  </si>
+  <si>
+    <t>Software accuracy</t>
   </si>
 </sst>
 </file>
@@ -1489,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T145"/>
+  <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -1566,16 +1566,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>94</v>
       </c>
       <c r="N3" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S3" s="32" t="s">
         <v>50</v>
@@ -1764,13 +1764,13 @@
       <c r="H8" s="26"/>
       <c r="I8" s="27"/>
       <c r="J8" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>90</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>89</v>
@@ -1883,21 +1883,10 @@
       <c r="H11" s="38">
         <v>3.2916666666666498E-3</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0</v>
-      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="6"/>
       <c r="S11" s="2">
         <v>21</v>
       </c>
@@ -2082,7 +2071,7 @@
         <v>82</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="7" t="s">
@@ -2167,7 +2156,7 @@
         <v>66</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7" t="s">
@@ -2201,7 +2190,7 @@
         <v>30</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L19" s="7"/>
       <c r="M19" s="7" t="s">
@@ -2359,7 +2348,7 @@
         <v>32</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6" t="s">
@@ -2420,7 +2409,7 @@
         <v>75</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6" t="s">
@@ -2532,7 +2521,7 @@
         <v>70</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L28" s="6"/>
       <c r="M28" s="6" t="s">
@@ -2559,7 +2548,7 @@
         <v>77</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6" t="s">
@@ -2647,7 +2636,7 @@
         <v>90</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M31" s="6" t="s">
         <v>91</v>
@@ -2700,9 +2689,8 @@
         <v>66</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L33" s="6"/>
+        <v>111</v>
+      </c>
       <c r="M33" s="6" t="s">
         <v>89</v>
       </c>
@@ -2751,13 +2739,13 @@
         <v>41</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K35" s="6" t="s">
         <v>92</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>89</v>
@@ -2873,13 +2861,13 @@
       </c>
       <c r="I38" s="27"/>
       <c r="J38" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K38" s="7" t="s">
         <v>92</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M38" s="7" t="s">
         <v>89</v>
@@ -2964,7 +2952,7 @@
         <v>66</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L40" s="8"/>
       <c r="M40" s="8" t="s">
@@ -2998,7 +2986,7 @@
         <v>41</v>
       </c>
       <c r="K41" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L41" s="18"/>
       <c r="M41" s="8" t="s">
@@ -3044,7 +3032,7 @@
         <v>46</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L42" s="7"/>
       <c r="M42" s="7" t="s">
@@ -3109,10 +3097,10 @@
       </c>
       <c r="I44" s="36"/>
       <c r="J44" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L44" s="8"/>
       <c r="M44" s="8" t="s">
@@ -3158,7 +3146,7 @@
         <v>49</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L45" s="7"/>
       <c r="M45" s="7" t="s">
@@ -3373,7 +3361,7 @@
         <v>90</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M50" s="8" t="s">
         <v>89</v>
@@ -3409,7 +3397,7 @@
         <v>92</v>
       </c>
       <c r="L51" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M51" s="8" t="s">
         <v>89</v>
@@ -3439,7 +3427,7 @@
       <c r="H52" s="35"/>
       <c r="I52" s="36"/>
       <c r="J52" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K52" s="8" t="s">
         <v>92</v>
@@ -3601,7 +3589,7 @@
         <v>77</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L56" s="7"/>
       <c r="M56" s="7" t="s">
@@ -3632,7 +3620,7 @@
       <c r="H57" s="26"/>
       <c r="I57" s="27"/>
       <c r="J57" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K57" s="7" t="s">
         <v>90</v>
@@ -4331,13 +4319,13 @@
       <c r="H76" s="26"/>
       <c r="I76" s="27"/>
       <c r="J76" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K76" s="7" t="s">
         <v>97</v>
       </c>
       <c r="L76" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M76" s="7" t="s">
         <v>89</v>
@@ -4674,7 +4662,7 @@
         <v>92</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M85" s="8" t="s">
         <v>89</v>
@@ -4834,10 +4822,10 @@
         <v>25</v>
       </c>
       <c r="K89" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L89" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M89" s="7" t="s">
         <v>89</v>
@@ -4940,10 +4928,10 @@
         <v>27</v>
       </c>
       <c r="K92" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L92" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M92" s="6" t="s">
         <v>89</v>
@@ -4988,7 +4976,7 @@
         <v>97</v>
       </c>
       <c r="L93" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M93" s="7" t="s">
         <v>89</v>
@@ -5018,10 +5006,10 @@
         <v>29</v>
       </c>
       <c r="K94" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L94" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M94" s="7" t="s">
         <v>89</v>
@@ -5107,72 +5095,69 @@
         <v>36</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:19" s="58" customFormat="1" ht="46" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>94</v>
       </c>
-      <c r="B97" s="3">
-        <v>32</v>
-      </c>
-      <c r="C97" s="33">
-        <v>1</v>
-      </c>
-      <c r="D97" s="34">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="E97" s="35">
-        <v>1.5074999999999899E-2</v>
-      </c>
-      <c r="F97" s="34">
-        <v>1</v>
-      </c>
-      <c r="G97" s="34">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="H97" s="35">
-        <v>1.5074999999999899E-2</v>
-      </c>
-      <c r="I97" s="36"/>
-      <c r="J97" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K97" s="8" t="s">
+      <c r="B97" s="23">
+        <v>30</v>
+      </c>
+      <c r="C97" s="24"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="26"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="25"/>
+      <c r="H97" s="26"/>
+      <c r="I97" s="27"/>
+      <c r="J97" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K97" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L97" s="8"/>
-      <c r="M97" s="8" t="s">
+      <c r="L97" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M97" s="7" t="s">
         <v>89</v>
       </c>
       <c r="N97" s="2">
         <v>1</v>
       </c>
-      <c r="S97" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="98" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>95</v>
       </c>
       <c r="B98" s="3">
         <v>32</v>
       </c>
-      <c r="C98" s="33"/>
-      <c r="D98" s="34"/>
-      <c r="E98" s="35"/>
-      <c r="F98" s="34"/>
-      <c r="G98" s="34"/>
-      <c r="H98" s="35"/>
+      <c r="C98" s="33">
+        <v>1</v>
+      </c>
+      <c r="D98" s="34">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="E98" s="35">
+        <v>1.5074999999999899E-2</v>
+      </c>
+      <c r="F98" s="34">
+        <v>1</v>
+      </c>
+      <c r="G98" s="34">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="H98" s="35">
+        <v>1.5074999999999899E-2</v>
+      </c>
       <c r="I98" s="36"/>
       <c r="J98" s="8" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="K98" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="L98" s="8" t="s">
-        <v>117</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="L98" s="8"/>
       <c r="M98" s="8" t="s">
         <v>89</v>
       </c>
@@ -5183,47 +5168,37 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>96</v>
       </c>
-      <c r="B99" s="23">
-        <v>33</v>
-      </c>
-      <c r="C99" s="24">
-        <v>1</v>
-      </c>
-      <c r="D99" s="25">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="E99" s="26">
-        <v>1.1375E-2</v>
-      </c>
-      <c r="F99" s="25">
-        <v>1</v>
-      </c>
-      <c r="G99" s="25">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="H99" s="26">
-        <v>1.1375E-2</v>
-      </c>
-      <c r="I99" s="27"/>
-      <c r="J99" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K99" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="L99" s="7"/>
-      <c r="M99" s="7" t="s">
+      <c r="B99" s="3">
+        <v>32</v>
+      </c>
+      <c r="C99" s="33"/>
+      <c r="D99" s="34"/>
+      <c r="E99" s="35"/>
+      <c r="F99" s="34"/>
+      <c r="G99" s="34"/>
+      <c r="H99" s="35"/>
+      <c r="I99" s="36"/>
+      <c r="J99" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K99" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L99" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="M99" s="8" t="s">
         <v>89</v>
       </c>
       <c r="N99" s="2">
         <v>1</v>
       </c>
       <c r="S99" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.35">
@@ -5233,15 +5208,27 @@
       <c r="B100" s="23">
         <v>33</v>
       </c>
-      <c r="C100" s="24"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="26"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
-      <c r="H100" s="26"/>
+      <c r="C100" s="24">
+        <v>1</v>
+      </c>
+      <c r="D100" s="25">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E100" s="26">
+        <v>1.1375E-2</v>
+      </c>
+      <c r="F100" s="25">
+        <v>1</v>
+      </c>
+      <c r="G100" s="25">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="H100" s="26">
+        <v>1.1375E-2</v>
+      </c>
       <c r="I100" s="27"/>
       <c r="J100" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K100" s="7" t="s">
         <v>90</v>
@@ -5261,42 +5248,31 @@
       <c r="A101" s="2">
         <v>98</v>
       </c>
-      <c r="B101" s="2">
-        <v>35</v>
-      </c>
-      <c r="C101" s="28">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="D101" s="37">
-        <v>0.4</v>
-      </c>
-      <c r="E101" s="38">
-        <v>2.30499999999999E-2</v>
-      </c>
-      <c r="F101" s="37">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="G101" s="37">
-        <v>0.4</v>
-      </c>
-      <c r="H101" s="38">
-        <v>2.30499999999999E-2</v>
-      </c>
-      <c r="J101" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K101" s="6" t="s">
+      <c r="B101" s="23">
+        <v>33</v>
+      </c>
+      <c r="C101" s="24"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="26"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="25"/>
+      <c r="H101" s="26"/>
+      <c r="I101" s="27"/>
+      <c r="J101" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K101" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L101" s="6"/>
-      <c r="M101" s="6" t="s">
+      <c r="L101" s="7"/>
+      <c r="M101" s="7" t="s">
         <v>89</v>
       </c>
       <c r="N101" s="2">
         <v>1</v>
       </c>
       <c r="S101" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.35">
@@ -5306,8 +5282,26 @@
       <c r="B102" s="2">
         <v>35</v>
       </c>
+      <c r="C102" s="28">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="D102" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="E102" s="38">
+        <v>2.30499999999999E-2</v>
+      </c>
+      <c r="F102" s="37">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G102" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="H102" s="38">
+        <v>2.30499999999999E-2</v>
+      </c>
       <c r="J102" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K102" s="6" t="s">
         <v>90</v>
@@ -5323,72 +5317,65 @@
         <v>41</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="46" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>100</v>
       </c>
-      <c r="B103" s="23">
-        <v>43</v>
-      </c>
-      <c r="C103" s="24">
-        <v>1</v>
-      </c>
-      <c r="D103" s="25">
-        <v>0.45</v>
-      </c>
-      <c r="E103" s="26">
-        <v>1.1925E-2</v>
-      </c>
-      <c r="F103" s="25">
-        <v>1</v>
-      </c>
-      <c r="G103" s="25">
-        <v>0.45</v>
-      </c>
-      <c r="H103" s="26">
-        <v>1.1925E-2</v>
-      </c>
-      <c r="I103" s="27"/>
-      <c r="J103" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K103" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="L103" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="M103" s="7" t="s">
+      <c r="B103" s="2">
+        <v>35</v>
+      </c>
+      <c r="J103" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K103" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6" t="s">
         <v>89</v>
       </c>
       <c r="N103" s="2">
         <v>1</v>
       </c>
       <c r="S103" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" ht="46" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>101</v>
       </c>
       <c r="B104" s="23">
         <v>43</v>
       </c>
-      <c r="C104" s="24"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="26"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="25"/>
-      <c r="H104" s="26"/>
+      <c r="C104" s="24">
+        <v>1</v>
+      </c>
+      <c r="D104" s="25">
+        <v>0.45</v>
+      </c>
+      <c r="E104" s="26">
+        <v>1.1925E-2</v>
+      </c>
+      <c r="F104" s="25">
+        <v>1</v>
+      </c>
+      <c r="G104" s="25">
+        <v>0.45</v>
+      </c>
+      <c r="H104" s="26">
+        <v>1.1925E-2</v>
+      </c>
       <c r="I104" s="27"/>
       <c r="J104" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="K104" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="L104" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="L104" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="M104" s="7" t="s">
         <v>89</v>
       </c>
@@ -5403,43 +5390,31 @@
       <c r="A105" s="2">
         <v>102</v>
       </c>
-      <c r="B105" s="3">
-        <v>46</v>
-      </c>
-      <c r="C105" s="33">
-        <v>1</v>
-      </c>
-      <c r="D105" s="34">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="E105" s="35">
-        <v>1.2075000000000001E-2</v>
-      </c>
-      <c r="F105" s="34">
-        <v>1</v>
-      </c>
-      <c r="G105" s="34">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="H105" s="35">
-        <v>1.2075000000000001E-2</v>
-      </c>
-      <c r="I105" s="36"/>
-      <c r="J105" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K105" s="8" t="s">
+      <c r="B105" s="23">
+        <v>43</v>
+      </c>
+      <c r="C105" s="24"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="26"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="25"/>
+      <c r="H105" s="26"/>
+      <c r="I105" s="27"/>
+      <c r="J105" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K105" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L105" s="8"/>
-      <c r="M105" s="8" t="s">
+      <c r="L105" s="7"/>
+      <c r="M105" s="7" t="s">
         <v>89</v>
       </c>
       <c r="N105" s="2">
         <v>1</v>
       </c>
       <c r="S105" s="2">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.35">
@@ -5449,15 +5424,27 @@
       <c r="B106" s="3">
         <v>46</v>
       </c>
-      <c r="C106" s="33"/>
-      <c r="D106" s="34"/>
-      <c r="E106" s="35"/>
-      <c r="F106" s="34"/>
-      <c r="G106" s="34"/>
-      <c r="H106" s="35"/>
+      <c r="C106" s="33">
+        <v>1</v>
+      </c>
+      <c r="D106" s="34">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E106" s="35">
+        <v>1.2075000000000001E-2</v>
+      </c>
+      <c r="F106" s="34">
+        <v>1</v>
+      </c>
+      <c r="G106" s="34">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="H106" s="35">
+        <v>1.2075000000000001E-2</v>
+      </c>
       <c r="I106" s="36"/>
       <c r="J106" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K106" s="8" t="s">
         <v>90</v>
@@ -5473,7 +5460,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>104</v>
       </c>
@@ -5488,14 +5475,12 @@
       <c r="H107" s="35"/>
       <c r="I107" s="36"/>
       <c r="J107" s="8" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="K107" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="L107" s="8" t="s">
-        <v>117</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="L107" s="8"/>
       <c r="M107" s="8" t="s">
         <v>89</v>
       </c>
@@ -5506,111 +5491,111 @@
         <v>54</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>105</v>
       </c>
-      <c r="B108" s="23">
-        <v>49</v>
-      </c>
-      <c r="C108" s="24">
-        <v>1</v>
-      </c>
-      <c r="D108" s="25">
-        <v>1</v>
-      </c>
-      <c r="E108" s="26">
-        <v>2.3249999999999898E-3</v>
-      </c>
-      <c r="F108" s="25">
-        <v>1</v>
-      </c>
-      <c r="G108" s="25">
-        <v>1</v>
-      </c>
-      <c r="H108" s="26">
-        <v>2.3249999999999898E-3</v>
-      </c>
-      <c r="I108" s="27"/>
-      <c r="J108" s="7"/>
-      <c r="K108" s="7"/>
-      <c r="L108" s="7"/>
-      <c r="M108" s="7"/>
+      <c r="B108" s="3">
+        <v>46</v>
+      </c>
+      <c r="C108" s="33"/>
+      <c r="D108" s="34"/>
+      <c r="E108" s="35"/>
+      <c r="F108" s="34"/>
+      <c r="G108" s="34"/>
+      <c r="H108" s="35"/>
+      <c r="I108" s="36"/>
+      <c r="J108" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K108" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L108" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="M108" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="N108" s="2">
         <v>1</v>
       </c>
       <c r="S108" s="2">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>106</v>
       </c>
-      <c r="B109" s="3">
-        <v>50</v>
-      </c>
-      <c r="C109" s="33">
-        <v>1</v>
-      </c>
-      <c r="D109" s="34">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="E109" s="35">
-        <v>1.7399999999999999E-2</v>
-      </c>
-      <c r="F109" s="34">
-        <v>1</v>
-      </c>
-      <c r="G109" s="34">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="H109" s="35">
-        <v>1.7399999999999999E-2</v>
-      </c>
-      <c r="I109" s="36"/>
-      <c r="J109" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K109" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L109" s="8"/>
-      <c r="M109" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="B109" s="23">
+        <v>49</v>
+      </c>
+      <c r="C109" s="24">
+        <v>1</v>
+      </c>
+      <c r="D109" s="25">
+        <v>1</v>
+      </c>
+      <c r="E109" s="26">
+        <v>2.3249999999999898E-3</v>
+      </c>
+      <c r="F109" s="25">
+        <v>1</v>
+      </c>
+      <c r="G109" s="25">
+        <v>1</v>
+      </c>
+      <c r="H109" s="26">
+        <v>2.3249999999999898E-3</v>
+      </c>
+      <c r="I109" s="27"/>
+      <c r="J109" s="7"/>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="7"/>
       <c r="N109" s="2">
         <v>1</v>
       </c>
       <c r="S109" s="2">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="110" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>107</v>
       </c>
       <c r="B110" s="3">
         <v>50</v>
       </c>
-      <c r="C110" s="41"/>
-      <c r="D110" s="42"/>
-      <c r="E110" s="43"/>
-      <c r="F110" s="42"/>
-      <c r="G110" s="42"/>
-      <c r="H110" s="43"/>
-      <c r="I110" s="44"/>
-      <c r="J110" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="K110" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="L110" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="M110" s="19" t="s">
-        <v>91</v>
+      <c r="C110" s="33">
+        <v>1</v>
+      </c>
+      <c r="D110" s="34">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="E110" s="35">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="F110" s="34">
+        <v>1</v>
+      </c>
+      <c r="G110" s="34">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="H110" s="35">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="I110" s="36"/>
+      <c r="J110" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K110" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L110" s="8"/>
+      <c r="M110" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="N110" s="2">
         <v>1</v>
@@ -5619,117 +5604,119 @@
         <v>59</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>108</v>
       </c>
-      <c r="B111" s="50">
-        <v>51</v>
-      </c>
-      <c r="C111" s="51">
-        <v>0.625</v>
-      </c>
-      <c r="D111" s="52">
-        <v>0.125</v>
-      </c>
-      <c r="E111" s="53">
-        <v>0.16375000000000001</v>
-      </c>
-      <c r="F111" s="52">
-        <v>0.625</v>
-      </c>
-      <c r="G111" s="52">
-        <v>0.125</v>
-      </c>
-      <c r="H111" s="53">
-        <v>0.16375000000000001</v>
-      </c>
-      <c r="I111" s="54"/>
-      <c r="J111" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="K111" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="L111" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="M111" s="20" t="s">
-        <v>89</v>
+      <c r="B111" s="3">
+        <v>50</v>
+      </c>
+      <c r="C111" s="41"/>
+      <c r="D111" s="42"/>
+      <c r="E111" s="43"/>
+      <c r="F111" s="42"/>
+      <c r="G111" s="42"/>
+      <c r="H111" s="43"/>
+      <c r="I111" s="44"/>
+      <c r="J111" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="K111" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="L111" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="M111" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="N111" s="2">
         <v>1</v>
       </c>
       <c r="S111" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>109</v>
       </c>
-      <c r="B112" s="3">
-        <v>52</v>
-      </c>
-      <c r="C112" s="33">
-        <v>0.9</v>
-      </c>
-      <c r="D112" s="34">
-        <v>0.25</v>
-      </c>
-      <c r="E112" s="35">
-        <v>2.2824999999999901E-2</v>
-      </c>
-      <c r="F112" s="34">
-        <v>1</v>
-      </c>
-      <c r="G112" s="34">
-        <v>1</v>
-      </c>
-      <c r="H112" s="35">
-        <v>3.1749999999999899E-3</v>
-      </c>
-      <c r="I112" s="36"/>
-      <c r="J112" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K112" s="8" t="s">
+      <c r="B112" s="50">
+        <v>51</v>
+      </c>
+      <c r="C112" s="51">
+        <v>0.625</v>
+      </c>
+      <c r="D112" s="52">
+        <v>0.125</v>
+      </c>
+      <c r="E112" s="53">
+        <v>0.16375000000000001</v>
+      </c>
+      <c r="F112" s="52">
+        <v>0.625</v>
+      </c>
+      <c r="G112" s="52">
+        <v>0.125</v>
+      </c>
+      <c r="H112" s="53">
+        <v>0.16375000000000001</v>
+      </c>
+      <c r="I112" s="54"/>
+      <c r="J112" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K112" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="L112" s="8"/>
-      <c r="M112" s="8" t="s">
-        <v>88</v>
+      <c r="L112" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="M112" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="N112" s="2">
         <v>1</v>
       </c>
       <c r="S112" s="2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="113" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>110</v>
       </c>
       <c r="B113" s="3">
         <v>52</v>
       </c>
-      <c r="C113" s="33"/>
-      <c r="D113" s="34"/>
-      <c r="E113" s="35"/>
-      <c r="F113" s="34"/>
-      <c r="G113" s="34"/>
-      <c r="H113" s="35"/>
+      <c r="C113" s="33">
+        <v>0.9</v>
+      </c>
+      <c r="D113" s="34">
+        <v>0.25</v>
+      </c>
+      <c r="E113" s="35">
+        <v>2.2824999999999901E-2</v>
+      </c>
+      <c r="F113" s="34">
+        <v>1</v>
+      </c>
+      <c r="G113" s="34">
+        <v>1</v>
+      </c>
+      <c r="H113" s="35">
+        <v>3.1749999999999899E-3</v>
+      </c>
       <c r="I113" s="36"/>
       <c r="J113" s="8" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="K113" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="L113" s="8"/>
-      <c r="M113" s="18" t="s">
-        <v>89</v>
+      <c r="M113" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="N113" s="2">
         <v>1</v>
@@ -5738,7 +5725,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="46" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>111</v>
       </c>
@@ -5753,15 +5740,13 @@
       <c r="H114" s="35"/>
       <c r="I114" s="36"/>
       <c r="J114" s="8" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="K114" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L114" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="M114" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L114" s="8"/>
+      <c r="M114" s="18" t="s">
         <v>89</v>
       </c>
       <c r="N114" s="2">
@@ -5771,7 +5756,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:19" ht="46" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>112</v>
       </c>
@@ -5785,13 +5770,15 @@
       <c r="G115" s="34"/>
       <c r="H115" s="35"/>
       <c r="I115" s="36"/>
-      <c r="J115" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="K115" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="L115" s="18"/>
+      <c r="J115" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K115" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L115" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="M115" s="8" t="s">
         <v>89</v>
       </c>
@@ -5806,68 +5793,66 @@
       <c r="A116" s="2">
         <v>113</v>
       </c>
-      <c r="B116" s="23">
-        <v>54</v>
-      </c>
-      <c r="C116" s="24">
-        <v>1</v>
-      </c>
-      <c r="D116" s="25">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="E116" s="26">
-        <v>1.05025E-2</v>
-      </c>
-      <c r="F116" s="25">
-        <v>1</v>
-      </c>
-      <c r="G116" s="25">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="H116" s="26">
-        <v>1.05025E-2</v>
-      </c>
-      <c r="I116" s="27"/>
-      <c r="J116" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="K116" s="7" t="s">
+      <c r="B116" s="3">
+        <v>52</v>
+      </c>
+      <c r="C116" s="33"/>
+      <c r="D116" s="34"/>
+      <c r="E116" s="35"/>
+      <c r="F116" s="34"/>
+      <c r="G116" s="34"/>
+      <c r="H116" s="35"/>
+      <c r="I116" s="36"/>
+      <c r="J116" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K116" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="L116" s="7"/>
-      <c r="M116" s="7" t="s">
+      <c r="L116" s="18"/>
+      <c r="M116" s="8" t="s">
         <v>89</v>
       </c>
       <c r="N116" s="2">
         <v>1</v>
       </c>
       <c r="S116" s="2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="117" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A117" s="2">
         <v>114</v>
       </c>
       <c r="B117" s="23">
         <v>54</v>
       </c>
-      <c r="C117" s="24"/>
-      <c r="D117" s="25"/>
-      <c r="E117" s="26"/>
-      <c r="F117" s="25"/>
-      <c r="G117" s="25"/>
-      <c r="H117" s="26"/>
+      <c r="C117" s="24">
+        <v>1</v>
+      </c>
+      <c r="D117" s="25">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E117" s="26">
+        <v>1.05025E-2</v>
+      </c>
+      <c r="F117" s="25">
+        <v>1</v>
+      </c>
+      <c r="G117" s="25">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="H117" s="26">
+        <v>1.05025E-2</v>
+      </c>
       <c r="I117" s="27"/>
       <c r="J117" s="7" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="K117" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="L117" s="7" t="s">
-        <v>122</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="L117" s="7"/>
       <c r="M117" s="7" t="s">
         <v>89</v>
       </c>
@@ -5882,87 +5867,77 @@
       <c r="A118" s="2">
         <v>115</v>
       </c>
-      <c r="B118" s="2">
-        <v>55</v>
-      </c>
-      <c r="C118" s="28">
-        <v>1</v>
-      </c>
-      <c r="D118" s="37">
-        <v>0.8</v>
-      </c>
-      <c r="E118" s="38">
-        <v>5.4750000000000198E-3</v>
-      </c>
-      <c r="F118" s="37">
-        <v>1</v>
-      </c>
-      <c r="G118" s="37">
-        <v>0.8</v>
-      </c>
-      <c r="H118" s="38">
-        <v>5.4750000000000198E-3</v>
-      </c>
-      <c r="J118" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K118" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L118" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="M118" s="6" t="s">
+      <c r="B118" s="23">
+        <v>54</v>
+      </c>
+      <c r="C118" s="24"/>
+      <c r="D118" s="25"/>
+      <c r="E118" s="26"/>
+      <c r="F118" s="25"/>
+      <c r="G118" s="25"/>
+      <c r="H118" s="26"/>
+      <c r="I118" s="27"/>
+      <c r="J118" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K118" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L118" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="M118" s="7" t="s">
         <v>89</v>
       </c>
       <c r="N118" s="2">
         <v>1</v>
       </c>
       <c r="S118" s="2">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A119" s="2">
         <v>116</v>
       </c>
-      <c r="B119" s="23">
-        <v>57</v>
-      </c>
-      <c r="C119" s="24">
-        <v>1</v>
-      </c>
-      <c r="D119" s="25">
+      <c r="B119" s="2">
+        <v>55</v>
+      </c>
+      <c r="C119" s="28">
+        <v>1</v>
+      </c>
+      <c r="D119" s="37">
         <v>0.8</v>
       </c>
-      <c r="E119" s="26">
-        <v>6.2999999999999801E-3</v>
-      </c>
-      <c r="F119" s="25">
-        <v>1</v>
-      </c>
-      <c r="G119" s="25">
+      <c r="E119" s="38">
+        <v>5.4750000000000198E-3</v>
+      </c>
+      <c r="F119" s="37">
+        <v>1</v>
+      </c>
+      <c r="G119" s="37">
         <v>0.8</v>
       </c>
-      <c r="H119" s="26">
-        <v>6.2999999999999801E-3</v>
-      </c>
-      <c r="I119" s="27"/>
-      <c r="J119" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K119" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="L119" s="7"/>
-      <c r="M119" s="7" t="s">
+      <c r="H119" s="38">
+        <v>5.4750000000000198E-3</v>
+      </c>
+      <c r="J119" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K119" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L119" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M119" s="6" t="s">
         <v>89</v>
       </c>
       <c r="N119" s="2">
         <v>1</v>
       </c>
       <c r="S119" s="2">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.35">
@@ -5972,267 +5947,277 @@
       <c r="B120" s="23">
         <v>57</v>
       </c>
-      <c r="C120" s="24"/>
-      <c r="D120" s="25"/>
-      <c r="E120" s="26"/>
-      <c r="F120" s="25"/>
-      <c r="G120" s="25"/>
-      <c r="H120" s="26"/>
+      <c r="C120" s="24">
+        <v>1</v>
+      </c>
+      <c r="D120" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="E120" s="26">
+        <v>6.2999999999999801E-3</v>
+      </c>
+      <c r="F120" s="25">
+        <v>1</v>
+      </c>
+      <c r="G120" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="H120" s="26">
+        <v>6.2999999999999801E-3</v>
+      </c>
       <c r="I120" s="27"/>
       <c r="J120" s="7" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="K120" s="7" t="s">
         <v>90</v>
       </c>
       <c r="L120" s="7"/>
-      <c r="M120" s="7"/>
+      <c r="M120" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="N120" s="2">
         <v>1</v>
+      </c>
+      <c r="S120" s="2">
+        <v>68</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>118</v>
       </c>
-      <c r="B121" s="3">
-        <v>58</v>
-      </c>
-      <c r="C121" s="33">
-        <v>1</v>
-      </c>
-      <c r="D121" s="34">
-        <v>0.8</v>
-      </c>
-      <c r="E121" s="35">
-        <v>6.2999999999999801E-3</v>
-      </c>
-      <c r="F121" s="34">
-        <v>1</v>
-      </c>
-      <c r="G121" s="34">
-        <v>0.8</v>
-      </c>
-      <c r="H121" s="35">
-        <v>6.2999999999999801E-3</v>
-      </c>
-      <c r="I121" s="36"/>
-      <c r="J121" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K121" s="8" t="s">
+      <c r="B121" s="23">
+        <v>57</v>
+      </c>
+      <c r="C121" s="24"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="26"/>
+      <c r="F121" s="25"/>
+      <c r="G121" s="25"/>
+      <c r="H121" s="26"/>
+      <c r="I121" s="27"/>
+      <c r="J121" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K121" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L121" s="8"/>
-      <c r="M121" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="L121" s="7"/>
+      <c r="M121" s="7"/>
       <c r="N121" s="2">
         <v>1</v>
       </c>
-      <c r="S121" s="2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="122" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>119</v>
       </c>
-      <c r="B122" s="23">
-        <v>59</v>
-      </c>
-      <c r="C122" s="24">
-        <v>0.4</v>
-      </c>
-      <c r="D122" s="25">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E122" s="26">
-        <v>0.1275</v>
-      </c>
-      <c r="F122" s="25">
-        <v>0.4</v>
-      </c>
-      <c r="G122" s="25">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H122" s="26">
-        <v>0.1275</v>
-      </c>
-      <c r="I122" s="27"/>
-      <c r="J122" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K122" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="L122" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="M122" s="7" t="s">
+      <c r="B122" s="3">
+        <v>58</v>
+      </c>
+      <c r="C122" s="33">
+        <v>1</v>
+      </c>
+      <c r="D122" s="34">
+        <v>0.8</v>
+      </c>
+      <c r="E122" s="35">
+        <v>6.2999999999999801E-3</v>
+      </c>
+      <c r="F122" s="34">
+        <v>1</v>
+      </c>
+      <c r="G122" s="34">
+        <v>0.8</v>
+      </c>
+      <c r="H122" s="35">
+        <v>6.2999999999999801E-3</v>
+      </c>
+      <c r="I122" s="36"/>
+      <c r="J122" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K122" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L122" s="8"/>
+      <c r="M122" s="8" t="s">
         <v>89</v>
       </c>
       <c r="N122" s="2">
         <v>1</v>
       </c>
       <c r="S122" s="2">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>120</v>
       </c>
-      <c r="B123" s="3">
-        <v>62</v>
-      </c>
-      <c r="C123" s="33">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="D123" s="34">
-        <v>0.375</v>
-      </c>
-      <c r="E123" s="35">
-        <v>2.1600000000000001E-2</v>
-      </c>
-      <c r="F123" s="34">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="G123" s="34">
-        <v>0.375</v>
-      </c>
-      <c r="H123" s="35">
-        <v>2.1600000000000001E-2</v>
-      </c>
-      <c r="I123" s="36"/>
-      <c r="J123" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="K123" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L123" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="M123" s="8" t="s">
+      <c r="B123" s="23">
+        <v>59</v>
+      </c>
+      <c r="C123" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="D123" s="25">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E123" s="26">
+        <v>0.1275</v>
+      </c>
+      <c r="F123" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="G123" s="25">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H123" s="26">
+        <v>0.1275</v>
+      </c>
+      <c r="I123" s="27"/>
+      <c r="J123" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K123" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L123" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M123" s="7" t="s">
         <v>89</v>
       </c>
       <c r="N123" s="2">
         <v>1</v>
       </c>
       <c r="S123" s="2">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>121</v>
       </c>
-      <c r="B124" s="23">
-        <v>67</v>
-      </c>
-      <c r="C124" s="24">
-        <v>0.6</v>
-      </c>
-      <c r="D124" s="25">
-        <v>0</v>
-      </c>
-      <c r="E124" s="26">
-        <v>0.15642500000000001</v>
-      </c>
-      <c r="F124" s="25">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="G124" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="H124" s="26">
-        <v>5.0774999999999897E-2</v>
-      </c>
-      <c r="I124" s="27"/>
-      <c r="J124" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="K124" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="L124" s="7"/>
-      <c r="M124" s="7" t="s">
-        <v>88</v>
+      <c r="B124" s="3">
+        <v>62</v>
+      </c>
+      <c r="C124" s="33">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D124" s="34">
+        <v>0.375</v>
+      </c>
+      <c r="E124" s="35">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="F124" s="34">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G124" s="34">
+        <v>0.375</v>
+      </c>
+      <c r="H124" s="35">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="I124" s="36"/>
+      <c r="J124" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K124" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L124" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="M124" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="N124" s="2">
         <v>1</v>
       </c>
       <c r="S124" s="2">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>122</v>
       </c>
-      <c r="B125" s="3">
-        <v>68</v>
-      </c>
-      <c r="C125" s="33">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="D125" s="34">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="E125" s="35">
-        <v>2.1524999999999999E-2</v>
-      </c>
-      <c r="F125" s="34">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="G125" s="34">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="H125" s="35">
-        <v>2.1524999999999999E-2</v>
-      </c>
-      <c r="I125" s="36"/>
-      <c r="J125" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="K125" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L125" s="8"/>
-      <c r="M125" s="8" t="s">
-        <v>89</v>
+      <c r="B125" s="23">
+        <v>67</v>
+      </c>
+      <c r="C125" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="D125" s="25">
+        <v>0</v>
+      </c>
+      <c r="E125" s="26">
+        <v>0.15642500000000001</v>
+      </c>
+      <c r="F125" s="25">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="G125" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="H125" s="26">
+        <v>5.0774999999999897E-2</v>
+      </c>
+      <c r="I125" s="27"/>
+      <c r="J125" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K125" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L125" s="7"/>
+      <c r="M125" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="N125" s="2">
         <v>1</v>
       </c>
       <c r="S125" s="2">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="126" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>123</v>
       </c>
       <c r="B126" s="3">
         <v>68</v>
       </c>
-      <c r="C126" s="33"/>
-      <c r="D126" s="34"/>
-      <c r="E126" s="35"/>
-      <c r="F126" s="34"/>
-      <c r="G126" s="34"/>
-      <c r="H126" s="35"/>
+      <c r="C126" s="33">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D126" s="34">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E126" s="35">
+        <v>2.1524999999999999E-2</v>
+      </c>
+      <c r="F126" s="34">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G126" s="34">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="H126" s="35">
+        <v>2.1524999999999999E-2</v>
+      </c>
       <c r="I126" s="36"/>
-      <c r="J126" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="K126" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="L126" s="18" t="s">
-        <v>124</v>
-      </c>
+      <c r="J126" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K126" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L126" s="8"/>
       <c r="M126" s="8" t="s">
         <v>89</v>
       </c>
@@ -6243,7 +6228,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>124</v>
       </c>
@@ -6258,12 +6243,14 @@
       <c r="H127" s="35"/>
       <c r="I127" s="36"/>
       <c r="J127" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K127" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="L127" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="L127" s="18" t="s">
+        <v>123</v>
+      </c>
       <c r="M127" s="8" t="s">
         <v>89</v>
       </c>
@@ -6278,43 +6265,31 @@
       <c r="A128" s="2">
         <v>125</v>
       </c>
-      <c r="B128" s="23">
-        <v>69</v>
-      </c>
-      <c r="C128" s="24">
-        <v>0.85</v>
-      </c>
-      <c r="D128" s="25">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="E128" s="26">
-        <v>2.81E-2</v>
-      </c>
-      <c r="F128" s="25">
-        <v>1</v>
-      </c>
-      <c r="G128" s="25">
-        <v>0.95</v>
-      </c>
-      <c r="H128" s="26">
-        <v>3.9749999999999803E-3</v>
-      </c>
-      <c r="I128" s="27"/>
-      <c r="J128" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K128" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="L128" s="7"/>
-      <c r="M128" s="7" t="s">
-        <v>88</v>
+      <c r="B128" s="3">
+        <v>68</v>
+      </c>
+      <c r="C128" s="33"/>
+      <c r="D128" s="34"/>
+      <c r="E128" s="35"/>
+      <c r="F128" s="34"/>
+      <c r="G128" s="34"/>
+      <c r="H128" s="35"/>
+      <c r="I128" s="36"/>
+      <c r="J128" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K128" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="L128" s="18"/>
+      <c r="M128" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="N128" s="2">
         <v>1</v>
       </c>
       <c r="S128" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.35">
@@ -6324,22 +6299,34 @@
       <c r="B129" s="23">
         <v>69</v>
       </c>
-      <c r="C129" s="51"/>
-      <c r="D129" s="52"/>
-      <c r="E129" s="53"/>
-      <c r="F129" s="52"/>
-      <c r="G129" s="52"/>
-      <c r="H129" s="53"/>
-      <c r="I129" s="54"/>
-      <c r="J129" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="K129" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="L129" s="20"/>
-      <c r="M129" s="20" t="s">
-        <v>89</v>
+      <c r="C129" s="24">
+        <v>0.85</v>
+      </c>
+      <c r="D129" s="25">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E129" s="26">
+        <v>2.81E-2</v>
+      </c>
+      <c r="F129" s="25">
+        <v>1</v>
+      </c>
+      <c r="G129" s="25">
+        <v>0.95</v>
+      </c>
+      <c r="H129" s="26">
+        <v>3.9749999999999803E-3</v>
+      </c>
+      <c r="I129" s="27"/>
+      <c r="J129" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K129" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L129" s="7"/>
+      <c r="M129" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="N129" s="2">
         <v>1</v>
@@ -6348,73 +6335,73 @@
         <v>83</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="46" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>127</v>
       </c>
-      <c r="B130" s="40">
-        <v>74</v>
-      </c>
-      <c r="C130" s="41">
-        <v>0.85</v>
-      </c>
-      <c r="D130" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="E130" s="43">
-        <v>3.8875E-2</v>
-      </c>
-      <c r="F130" s="42">
-        <v>0.85</v>
-      </c>
-      <c r="G130" s="42">
-        <v>0.15</v>
-      </c>
-      <c r="H130" s="43">
-        <v>3.8875E-2</v>
-      </c>
-      <c r="I130" s="44"/>
-      <c r="J130" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="K130" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="L130" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="M130" s="19" t="s">
+      <c r="B130" s="23">
+        <v>69</v>
+      </c>
+      <c r="C130" s="51"/>
+      <c r="D130" s="52"/>
+      <c r="E130" s="53"/>
+      <c r="F130" s="52"/>
+      <c r="G130" s="52"/>
+      <c r="H130" s="53"/>
+      <c r="I130" s="54"/>
+      <c r="J130" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="K130" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="L130" s="20"/>
+      <c r="M130" s="20" t="s">
         <v>89</v>
       </c>
       <c r="N130" s="2">
         <v>1</v>
       </c>
       <c r="S130" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" ht="46" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>128</v>
       </c>
       <c r="B131" s="40">
         <v>74</v>
       </c>
-      <c r="C131" s="33"/>
-      <c r="D131" s="34"/>
-      <c r="E131" s="35"/>
-      <c r="F131" s="34"/>
-      <c r="G131" s="34"/>
-      <c r="H131" s="35"/>
-      <c r="I131" s="36"/>
-      <c r="J131" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="K131" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="L131" s="8"/>
-      <c r="M131" s="8" t="s">
+      <c r="C131" s="41">
+        <v>0.85</v>
+      </c>
+      <c r="D131" s="42">
+        <v>0.15</v>
+      </c>
+      <c r="E131" s="43">
+        <v>3.8875E-2</v>
+      </c>
+      <c r="F131" s="42">
+        <v>0.85</v>
+      </c>
+      <c r="G131" s="42">
+        <v>0.15</v>
+      </c>
+      <c r="H131" s="43">
+        <v>3.8875E-2</v>
+      </c>
+      <c r="I131" s="44"/>
+      <c r="J131" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="K131" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="L131" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="M131" s="19" t="s">
         <v>89</v>
       </c>
       <c r="N131" s="2">
@@ -6428,68 +6415,66 @@
       <c r="A132" s="2">
         <v>129</v>
       </c>
-      <c r="B132" s="23">
-        <v>75</v>
-      </c>
-      <c r="C132" s="24">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="D132" s="25">
-        <v>0.45</v>
-      </c>
-      <c r="E132" s="26">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="F132" s="25">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="G132" s="25">
-        <v>0.45</v>
-      </c>
-      <c r="H132" s="26">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="I132" s="27"/>
-      <c r="J132" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="K132" s="7" t="s">
+      <c r="B132" s="40">
+        <v>74</v>
+      </c>
+      <c r="C132" s="33"/>
+      <c r="D132" s="34"/>
+      <c r="E132" s="35"/>
+      <c r="F132" s="34"/>
+      <c r="G132" s="34"/>
+      <c r="H132" s="35"/>
+      <c r="I132" s="36"/>
+      <c r="J132" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K132" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="L132" s="7"/>
-      <c r="M132" s="7" t="s">
+      <c r="L132" s="8"/>
+      <c r="M132" s="8" t="s">
         <v>89</v>
       </c>
       <c r="N132" s="2">
         <v>1</v>
       </c>
       <c r="S132" s="2">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="133" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A133" s="2">
         <v>130</v>
       </c>
       <c r="B133" s="23">
         <v>75</v>
       </c>
-      <c r="C133" s="24"/>
-      <c r="D133" s="25"/>
-      <c r="E133" s="26"/>
-      <c r="F133" s="25"/>
-      <c r="G133" s="25"/>
-      <c r="H133" s="26"/>
+      <c r="C133" s="24">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D133" s="25">
+        <v>0.45</v>
+      </c>
+      <c r="E133" s="26">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="F133" s="25">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G133" s="25">
+        <v>0.45</v>
+      </c>
+      <c r="H133" s="26">
+        <v>1.5625E-2</v>
+      </c>
       <c r="I133" s="27"/>
       <c r="J133" s="7" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="K133" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="L133" s="7" t="s">
-        <v>127</v>
-      </c>
+      <c r="L133" s="7"/>
       <c r="M133" s="7" t="s">
         <v>89</v>
       </c>
@@ -6500,46 +6485,37 @@
         <v>93</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>131</v>
       </c>
-      <c r="B134" s="2">
-        <v>77</v>
-      </c>
-      <c r="C134" s="28">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="D134" s="37">
-        <v>0</v>
-      </c>
-      <c r="E134" s="38">
-        <v>0.994475</v>
-      </c>
-      <c r="F134" s="37">
-        <v>1</v>
-      </c>
-      <c r="G134" s="37">
-        <v>0.625</v>
-      </c>
-      <c r="H134" s="38">
-        <v>8.4250000000000002E-3</v>
-      </c>
-      <c r="J134" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K134" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="L134" s="6"/>
-      <c r="M134" s="6" t="s">
-        <v>88</v>
+      <c r="B134" s="23">
+        <v>75</v>
+      </c>
+      <c r="C134" s="24"/>
+      <c r="D134" s="25"/>
+      <c r="E134" s="26"/>
+      <c r="F134" s="25"/>
+      <c r="G134" s="25"/>
+      <c r="H134" s="26"/>
+      <c r="I134" s="27"/>
+      <c r="J134" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K134" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L134" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="M134" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="N134" s="2">
         <v>1</v>
       </c>
       <c r="S134" s="2">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.35">
@@ -6549,15 +6525,33 @@
       <c r="B135" s="2">
         <v>77</v>
       </c>
+      <c r="C135" s="28">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D135" s="37">
+        <v>0</v>
+      </c>
+      <c r="E135" s="38">
+        <v>0.994475</v>
+      </c>
+      <c r="F135" s="37">
+        <v>1</v>
+      </c>
+      <c r="G135" s="37">
+        <v>0.625</v>
+      </c>
+      <c r="H135" s="38">
+        <v>8.4250000000000002E-3</v>
+      </c>
       <c r="J135" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K135" s="6" t="s">
-        <v>90</v>
+        <v>55</v>
+      </c>
+      <c r="K135" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="L135" s="6"/>
       <c r="M135" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N135" s="2">
         <v>1</v>
@@ -6566,7 +6560,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>133</v>
       </c>
@@ -6574,14 +6568,12 @@
         <v>77</v>
       </c>
       <c r="J136" s="6" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="K136" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L136" s="6" t="s">
-        <v>117</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="L136" s="6"/>
       <c r="M136" s="6" t="s">
         <v>89</v>
       </c>
@@ -6592,185 +6584,187 @@
         <v>95</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:19" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>134</v>
       </c>
-      <c r="B137" s="50">
-        <v>79</v>
-      </c>
-      <c r="C137" s="51">
-        <v>1</v>
-      </c>
-      <c r="D137" s="52">
-        <v>0.95</v>
-      </c>
-      <c r="E137" s="53">
-        <v>2.72499999999999E-3</v>
-      </c>
-      <c r="F137" s="52">
-        <v>1</v>
-      </c>
-      <c r="G137" s="52">
-        <v>0.95</v>
-      </c>
-      <c r="H137" s="53">
-        <v>2.72499999999999E-3</v>
-      </c>
-      <c r="I137" s="54"/>
-      <c r="J137" s="20"/>
-      <c r="K137" s="20"/>
-      <c r="L137" s="20"/>
-      <c r="M137" s="20"/>
+      <c r="B137" s="2">
+        <v>77</v>
+      </c>
+      <c r="J137" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K137" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="L137" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="M137" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="N137" s="2">
         <v>1</v>
       </c>
       <c r="S137" s="2">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>135</v>
       </c>
-      <c r="B138" s="3">
-        <v>80</v>
-      </c>
-      <c r="C138" s="33">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="D138" s="34">
-        <v>0.05</v>
-      </c>
-      <c r="E138" s="35">
-        <v>0.94814999999999905</v>
-      </c>
-      <c r="F138" s="34">
-        <v>1</v>
-      </c>
-      <c r="G138" s="34">
-        <v>1</v>
-      </c>
-      <c r="H138" s="35">
-        <v>1.89999999999999E-3</v>
-      </c>
-      <c r="I138" s="36"/>
-      <c r="J138" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K138" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="L138" s="8"/>
-      <c r="M138" s="8" t="s">
-        <v>88</v>
-      </c>
+      <c r="B138" s="50">
+        <v>79</v>
+      </c>
+      <c r="C138" s="51">
+        <v>1</v>
+      </c>
+      <c r="D138" s="52">
+        <v>0.95</v>
+      </c>
+      <c r="E138" s="53">
+        <v>2.72499999999999E-3</v>
+      </c>
+      <c r="F138" s="52">
+        <v>1</v>
+      </c>
+      <c r="G138" s="52">
+        <v>0.95</v>
+      </c>
+      <c r="H138" s="53">
+        <v>2.72499999999999E-3</v>
+      </c>
+      <c r="I138" s="54"/>
+      <c r="J138" s="20"/>
+      <c r="K138" s="20"/>
+      <c r="L138" s="20"/>
+      <c r="M138" s="20"/>
       <c r="N138" s="2">
         <v>1</v>
       </c>
       <c r="S138" s="2">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="139" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>136</v>
       </c>
-      <c r="B139" s="23">
-        <v>81</v>
-      </c>
-      <c r="C139" s="24">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="D139" s="25">
+      <c r="B139" s="3">
+        <v>80</v>
+      </c>
+      <c r="C139" s="33">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D139" s="34">
         <v>0.05</v>
       </c>
-      <c r="E139" s="26">
-        <v>0.11877500000000001</v>
-      </c>
-      <c r="F139" s="25">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="G139" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="H139" s="26">
-        <v>0.11877500000000001</v>
-      </c>
-      <c r="I139" s="27"/>
-      <c r="J139" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="K139" s="7" t="s">
+      <c r="E139" s="35">
+        <v>0.94814999999999905</v>
+      </c>
+      <c r="F139" s="34">
+        <v>1</v>
+      </c>
+      <c r="G139" s="34">
+        <v>1</v>
+      </c>
+      <c r="H139" s="35">
+        <v>1.89999999999999E-3</v>
+      </c>
+      <c r="I139" s="36"/>
+      <c r="J139" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K139" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="L139" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="M139" s="7" t="s">
-        <v>89</v>
+      <c r="L139" s="8"/>
+      <c r="M139" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="N139" s="2">
         <v>1</v>
       </c>
       <c r="S139" s="2">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="140" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A140" s="2">
         <v>137</v>
       </c>
-      <c r="B140" s="2">
-        <v>83</v>
-      </c>
-      <c r="C140" s="28">
-        <v>1</v>
-      </c>
-      <c r="D140" s="37">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="E140" s="38">
-        <v>6.6499999999999797E-3</v>
-      </c>
-      <c r="F140" s="37">
-        <v>1</v>
-      </c>
-      <c r="G140" s="37">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="H140" s="38">
-        <v>6.6499999999999797E-3</v>
-      </c>
-      <c r="J140" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K140" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="L140" s="10"/>
-      <c r="M140" s="6" t="s">
+      <c r="B140" s="23">
+        <v>81</v>
+      </c>
+      <c r="C140" s="24">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D140" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="E140" s="26">
+        <v>0.11877500000000001</v>
+      </c>
+      <c r="F140" s="25">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="G140" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="H140" s="26">
+        <v>0.11877500000000001</v>
+      </c>
+      <c r="I140" s="27"/>
+      <c r="J140" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="K140" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L140" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="M140" s="7" t="s">
         <v>89</v>
       </c>
       <c r="N140" s="2">
         <v>1</v>
       </c>
       <c r="S140" s="2">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" ht="23" x14ac:dyDescent="0.35">
       <c r="A141" s="2">
         <v>138</v>
       </c>
       <c r="B141" s="2">
         <v>83</v>
       </c>
+      <c r="C141" s="28">
+        <v>1</v>
+      </c>
+      <c r="D141" s="37">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E141" s="38">
+        <v>6.6499999999999797E-3</v>
+      </c>
+      <c r="F141" s="37">
+        <v>1</v>
+      </c>
+      <c r="G141" s="37">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H141" s="38">
+        <v>6.6499999999999797E-3</v>
+      </c>
       <c r="J141" s="10" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="K141" s="10" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="L141" s="10"/>
       <c r="M141" s="6" t="s">
@@ -6779,74 +6773,65 @@
       <c r="N141" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="S141" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A142" s="2">
         <v>139</v>
       </c>
-      <c r="B142" s="23">
-        <v>84</v>
-      </c>
-      <c r="C142" s="24">
-        <v>1</v>
-      </c>
-      <c r="D142" s="25">
-        <v>0.85</v>
-      </c>
-      <c r="E142" s="26">
-        <v>5.37499999999999E-3</v>
-      </c>
-      <c r="F142" s="25">
-        <v>1</v>
-      </c>
-      <c r="G142" s="25">
-        <v>0.85</v>
-      </c>
-      <c r="H142" s="26">
-        <v>5.37499999999999E-3</v>
-      </c>
-      <c r="I142" s="27"/>
-      <c r="J142" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="K142" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="L142" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="M142" s="7" t="s">
+      <c r="B142" s="2">
+        <v>83</v>
+      </c>
+      <c r="J142" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K142" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="L142" s="10"/>
+      <c r="M142" s="6" t="s">
         <v>89</v>
       </c>
       <c r="N142" s="2">
         <v>1</v>
       </c>
-      <c r="S142" s="2">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="143" spans="1:19" ht="46" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:19" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>140</v>
       </c>
       <c r="B143" s="23">
         <v>84</v>
       </c>
-      <c r="C143" s="24"/>
-      <c r="D143" s="25"/>
-      <c r="E143" s="26"/>
-      <c r="F143" s="25"/>
-      <c r="G143" s="25"/>
-      <c r="H143" s="26"/>
+      <c r="C143" s="24">
+        <v>1</v>
+      </c>
+      <c r="D143" s="25">
+        <v>0.85</v>
+      </c>
+      <c r="E143" s="26">
+        <v>5.37499999999999E-3</v>
+      </c>
+      <c r="F143" s="25">
+        <v>1</v>
+      </c>
+      <c r="G143" s="25">
+        <v>0.85</v>
+      </c>
+      <c r="H143" s="26">
+        <v>5.37499999999999E-3</v>
+      </c>
       <c r="I143" s="27"/>
-      <c r="J143" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="K143" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L143" s="9" t="s">
-        <v>129</v>
+      <c r="J143" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K143" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L143" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="M143" s="7" t="s">
         <v>89</v>
@@ -6858,76 +6843,109 @@
         <v>105</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:19" ht="46" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>141</v>
       </c>
-      <c r="B144" s="2">
-        <v>85</v>
-      </c>
-      <c r="C144" s="28">
-        <v>1</v>
-      </c>
-      <c r="D144" s="37">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="E144" s="38">
-        <v>6.02499999999998E-3</v>
-      </c>
-      <c r="F144" s="37">
-        <v>1</v>
-      </c>
-      <c r="G144" s="37">
-        <v>0.77500000000000002</v>
-      </c>
-      <c r="H144" s="38">
-        <v>6.02499999999998E-3</v>
-      </c>
-      <c r="J144" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K144" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L144" s="6"/>
-      <c r="M144" s="6" t="s">
+      <c r="B144" s="23">
+        <v>84</v>
+      </c>
+      <c r="C144" s="24"/>
+      <c r="D144" s="25"/>
+      <c r="E144" s="26"/>
+      <c r="F144" s="25"/>
+      <c r="G144" s="25"/>
+      <c r="H144" s="26"/>
+      <c r="I144" s="27"/>
+      <c r="J144" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K144" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="L144" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="M144" s="7" t="s">
         <v>89</v>
       </c>
       <c r="N144" s="2">
         <v>1</v>
       </c>
       <c r="S144" s="2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="145" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>142</v>
       </c>
       <c r="B145" s="2">
         <v>85</v>
       </c>
-      <c r="C145" s="39"/>
-      <c r="D145" s="55"/>
-      <c r="E145" s="56"/>
-      <c r="F145" s="55"/>
-      <c r="G145" s="55"/>
-      <c r="H145" s="56"/>
-      <c r="I145" s="57"/>
-      <c r="J145" s="21" t="s">
+      <c r="C145" s="28">
+        <v>1</v>
+      </c>
+      <c r="D145" s="37">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="E145" s="38">
+        <v>6.02499999999998E-3</v>
+      </c>
+      <c r="F145" s="37">
+        <v>1</v>
+      </c>
+      <c r="G145" s="37">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="H145" s="38">
+        <v>6.02499999999998E-3</v>
+      </c>
+      <c r="J145" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K145" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L145" s="6"/>
+      <c r="M145" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="N145" s="2">
+        <v>1</v>
+      </c>
+      <c r="S145" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" ht="23" x14ac:dyDescent="0.35">
+      <c r="A146" s="2">
+        <v>143</v>
+      </c>
+      <c r="B146" s="2">
+        <v>85</v>
+      </c>
+      <c r="C146" s="39"/>
+      <c r="D146" s="55"/>
+      <c r="E146" s="56"/>
+      <c r="F146" s="55"/>
+      <c r="G146" s="55"/>
+      <c r="H146" s="56"/>
+      <c r="I146" s="57"/>
+      <c r="J146" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="K145" s="21" t="s">
+      <c r="K146" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="L145" s="21"/>
-      <c r="M145" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="N145" s="2">
-        <v>1</v>
-      </c>
-      <c r="S145" s="2">
+      <c r="L146" s="21"/>
+      <c r="M146" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="N146" s="2">
+        <v>1</v>
+      </c>
+      <c r="S146" s="2">
         <v>106</v>
       </c>
     </row>

</xml_diff>